<commit_message>
Gantt optioinal part done
</commit_message>
<xml_diff>
--- a/Reuniones_Coordinacion/Diagrama_Gantt_8_4_25_Saul_Fernando_Raquel_Irene.xlsx
+++ b/Reuniones_Coordinacion/Diagrama_Gantt_8_4_25_Saul_Fernando_Raquel_Irene.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\saul\Pprog_conversation\Reuniones_Coordinacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFFCF521-2D65-4539-9BF5-D7F742740E61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10A0D736-C852-4EB4-8F18-26400B0440BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10960" xr2:uid="{76F30C29-DD84-4491-9B4C-00A38B383DA8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{76F30C29-DD84-4491-9B4C-00A38B383DA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="107">
   <si>
     <t>CRONOGRAMA I3</t>
   </si>
@@ -361,7 +362,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="25">
+  <fills count="26">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -506,6 +507,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="28">
     <border>
@@ -890,7 +897,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="116">
+  <cellXfs count="126">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1069,6 +1076,66 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1141,60 +1208,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1511,8 +1532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13B8C02F-838E-4995-8CF9-185661B72170}">
   <dimension ref="A1:AA66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="84" workbookViewId="0">
-      <selection activeCell="O43" sqref="O43"/>
+    <sheetView tabSelected="1" zoomScale="84" workbookViewId="0">
+      <selection activeCell="AC57" sqref="AC57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1525,114 +1546,114 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="78" t="s">
+      <c r="A1" s="98" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
-      <c r="I1" s="79"/>
-      <c r="J1" s="79"/>
-      <c r="K1" s="79"/>
-      <c r="L1" s="79"/>
-      <c r="M1" s="79"/>
-      <c r="N1" s="79"/>
-      <c r="O1" s="79"/>
-      <c r="P1" s="79"/>
-      <c r="Q1" s="79"/>
-      <c r="R1" s="79"/>
-      <c r="S1" s="79"/>
-      <c r="T1" s="79"/>
-      <c r="U1" s="79"/>
-      <c r="V1" s="79"/>
-      <c r="W1" s="79"/>
-      <c r="X1" s="79"/>
-      <c r="Y1" s="79"/>
-      <c r="Z1" s="79"/>
-      <c r="AA1" s="80"/>
+      <c r="B1" s="99"/>
+      <c r="C1" s="99"/>
+      <c r="D1" s="99"/>
+      <c r="E1" s="99"/>
+      <c r="F1" s="99"/>
+      <c r="G1" s="99"/>
+      <c r="H1" s="99"/>
+      <c r="I1" s="99"/>
+      <c r="J1" s="99"/>
+      <c r="K1" s="99"/>
+      <c r="L1" s="99"/>
+      <c r="M1" s="99"/>
+      <c r="N1" s="99"/>
+      <c r="O1" s="99"/>
+      <c r="P1" s="99"/>
+      <c r="Q1" s="99"/>
+      <c r="R1" s="99"/>
+      <c r="S1" s="99"/>
+      <c r="T1" s="99"/>
+      <c r="U1" s="99"/>
+      <c r="V1" s="99"/>
+      <c r="W1" s="99"/>
+      <c r="X1" s="99"/>
+      <c r="Y1" s="99"/>
+      <c r="Z1" s="99"/>
+      <c r="AA1" s="100"/>
     </row>
     <row r="2" spans="1:27" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="81" t="s">
+      <c r="A2" s="101" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="82"/>
-      <c r="C2" s="87" t="s">
+      <c r="B2" s="102"/>
+      <c r="C2" s="107" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="90" t="s">
+      <c r="D2" s="110" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90"/>
-      <c r="G2" s="91"/>
-      <c r="H2" s="94" t="s">
+      <c r="E2" s="110"/>
+      <c r="F2" s="110"/>
+      <c r="G2" s="111"/>
+      <c r="H2" s="114" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="90"/>
-      <c r="J2" s="90"/>
-      <c r="K2" s="90"/>
-      <c r="L2" s="90"/>
-      <c r="M2" s="90"/>
-      <c r="N2" s="90"/>
-      <c r="O2" s="90"/>
-      <c r="P2" s="90"/>
-      <c r="Q2" s="90"/>
-      <c r="R2" s="90"/>
-      <c r="S2" s="90"/>
-      <c r="T2" s="90"/>
-      <c r="U2" s="90"/>
-      <c r="V2" s="90"/>
-      <c r="W2" s="90"/>
-      <c r="X2" s="90"/>
-      <c r="Y2" s="90"/>
-      <c r="Z2" s="90"/>
-      <c r="AA2" s="95"/>
+      <c r="I2" s="110"/>
+      <c r="J2" s="110"/>
+      <c r="K2" s="110"/>
+      <c r="L2" s="110"/>
+      <c r="M2" s="110"/>
+      <c r="N2" s="110"/>
+      <c r="O2" s="110"/>
+      <c r="P2" s="110"/>
+      <c r="Q2" s="110"/>
+      <c r="R2" s="110"/>
+      <c r="S2" s="110"/>
+      <c r="T2" s="110"/>
+      <c r="U2" s="110"/>
+      <c r="V2" s="110"/>
+      <c r="W2" s="110"/>
+      <c r="X2" s="110"/>
+      <c r="Y2" s="110"/>
+      <c r="Z2" s="110"/>
+      <c r="AA2" s="115"/>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A3" s="83"/>
-      <c r="B3" s="84"/>
-      <c r="C3" s="88"/>
-      <c r="D3" s="92"/>
-      <c r="E3" s="92"/>
-      <c r="F3" s="92"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="96" t="s">
+      <c r="A3" s="103"/>
+      <c r="B3" s="104"/>
+      <c r="C3" s="108"/>
+      <c r="D3" s="112"/>
+      <c r="E3" s="112"/>
+      <c r="F3" s="112"/>
+      <c r="G3" s="113"/>
+      <c r="H3" s="116" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="92"/>
-      <c r="J3" s="92"/>
-      <c r="K3" s="92"/>
-      <c r="L3" s="92"/>
-      <c r="M3" s="92" t="s">
+      <c r="I3" s="112"/>
+      <c r="J3" s="112"/>
+      <c r="K3" s="112"/>
+      <c r="L3" s="112"/>
+      <c r="M3" s="112" t="s">
         <v>6</v>
       </c>
-      <c r="N3" s="92"/>
-      <c r="O3" s="92"/>
-      <c r="P3" s="92"/>
-      <c r="Q3" s="92"/>
-      <c r="R3" s="92" t="s">
+      <c r="N3" s="112"/>
+      <c r="O3" s="112"/>
+      <c r="P3" s="112"/>
+      <c r="Q3" s="112"/>
+      <c r="R3" s="112" t="s">
         <v>7</v>
       </c>
-      <c r="S3" s="92"/>
-      <c r="T3" s="92"/>
-      <c r="U3" s="92"/>
-      <c r="V3" s="92"/>
-      <c r="W3" s="92" t="s">
+      <c r="S3" s="112"/>
+      <c r="T3" s="112"/>
+      <c r="U3" s="112"/>
+      <c r="V3" s="112"/>
+      <c r="W3" s="112" t="s">
         <v>8</v>
       </c>
-      <c r="X3" s="92"/>
-      <c r="Y3" s="92"/>
-      <c r="Z3" s="92"/>
-      <c r="AA3" s="97"/>
+      <c r="X3" s="112"/>
+      <c r="Y3" s="112"/>
+      <c r="Z3" s="112"/>
+      <c r="AA3" s="117"/>
     </row>
     <row r="4" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="85"/>
-      <c r="B4" s="86"/>
-      <c r="C4" s="89"/>
+      <c r="A4" s="105"/>
+      <c r="B4" s="106"/>
+      <c r="C4" s="109"/>
       <c r="D4" s="70" t="s">
         <v>9</v>
       </c>
@@ -1771,21 +1792,21 @@
       <c r="I6" s="16"/>
       <c r="J6" s="16"/>
       <c r="K6" s="16"/>
-      <c r="L6" s="99"/>
-      <c r="M6" s="99"/>
-      <c r="N6" s="99"/>
-      <c r="O6" s="99"/>
-      <c r="P6" s="99"/>
-      <c r="Q6" s="99"/>
-      <c r="R6" s="99"/>
-      <c r="S6" s="99"/>
-      <c r="T6" s="99"/>
-      <c r="U6" s="99"/>
-      <c r="V6" s="99"/>
-      <c r="W6" s="99"/>
-      <c r="X6" s="99"/>
-      <c r="Y6" s="99"/>
-      <c r="Z6" s="99"/>
+      <c r="L6" s="75"/>
+      <c r="M6" s="75"/>
+      <c r="N6" s="75"/>
+      <c r="O6" s="75"/>
+      <c r="P6" s="75"/>
+      <c r="Q6" s="75"/>
+      <c r="R6" s="75"/>
+      <c r="S6" s="75"/>
+      <c r="T6" s="75"/>
+      <c r="U6" s="75"/>
+      <c r="V6" s="75"/>
+      <c r="W6" s="75"/>
+      <c r="X6" s="75"/>
+      <c r="Y6" s="75"/>
+      <c r="Z6" s="75"/>
       <c r="AA6" s="19"/>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.35">
@@ -1814,21 +1835,21 @@
       <c r="I7" s="16"/>
       <c r="J7" s="16"/>
       <c r="K7" s="16"/>
-      <c r="L7" s="99"/>
-      <c r="M7" s="99"/>
-      <c r="N7" s="99"/>
-      <c r="O7" s="99"/>
-      <c r="P7" s="99"/>
-      <c r="Q7" s="99"/>
-      <c r="R7" s="99"/>
-      <c r="S7" s="99"/>
-      <c r="T7" s="99"/>
-      <c r="U7" s="99"/>
-      <c r="V7" s="99"/>
-      <c r="W7" s="99"/>
-      <c r="X7" s="99"/>
-      <c r="Y7" s="99"/>
-      <c r="Z7" s="99"/>
+      <c r="L7" s="75"/>
+      <c r="M7" s="75"/>
+      <c r="N7" s="75"/>
+      <c r="O7" s="75"/>
+      <c r="P7" s="75"/>
+      <c r="Q7" s="75"/>
+      <c r="R7" s="75"/>
+      <c r="S7" s="75"/>
+      <c r="T7" s="75"/>
+      <c r="U7" s="75"/>
+      <c r="V7" s="75"/>
+      <c r="W7" s="75"/>
+      <c r="X7" s="75"/>
+      <c r="Y7" s="75"/>
+      <c r="Z7" s="75"/>
       <c r="AA7" s="19"/>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.35">
@@ -1857,21 +1878,21 @@
       <c r="I8" s="16"/>
       <c r="J8" s="16"/>
       <c r="K8" s="16"/>
-      <c r="L8" s="99"/>
-      <c r="M8" s="99"/>
-      <c r="N8" s="99"/>
-      <c r="O8" s="99"/>
-      <c r="P8" s="99"/>
-      <c r="Q8" s="99"/>
-      <c r="R8" s="99"/>
-      <c r="S8" s="99"/>
-      <c r="T8" s="99"/>
-      <c r="U8" s="99"/>
-      <c r="V8" s="99"/>
-      <c r="W8" s="99"/>
-      <c r="X8" s="99"/>
-      <c r="Y8" s="99"/>
-      <c r="Z8" s="99"/>
+      <c r="L8" s="75"/>
+      <c r="M8" s="75"/>
+      <c r="N8" s="75"/>
+      <c r="O8" s="75"/>
+      <c r="P8" s="75"/>
+      <c r="Q8" s="75"/>
+      <c r="R8" s="75"/>
+      <c r="S8" s="75"/>
+      <c r="T8" s="75"/>
+      <c r="U8" s="75"/>
+      <c r="V8" s="75"/>
+      <c r="W8" s="75"/>
+      <c r="X8" s="75"/>
+      <c r="Y8" s="75"/>
+      <c r="Z8" s="75"/>
       <c r="AA8" s="19"/>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.35">
@@ -1898,31 +1919,31 @@
       <c r="I9" s="16"/>
       <c r="J9" s="16"/>
       <c r="K9" s="16"/>
-      <c r="L9" s="100" t="s">
+      <c r="L9" s="76" t="s">
         <v>11</v>
       </c>
       <c r="M9" s="16"/>
       <c r="N9" s="16"/>
       <c r="O9" s="16"/>
       <c r="P9" s="16"/>
-      <c r="Q9" s="100" t="s">
+      <c r="Q9" s="76" t="s">
         <v>12</v>
       </c>
       <c r="R9" s="16"/>
       <c r="S9" s="16"/>
       <c r="T9" s="16"/>
       <c r="U9" s="16"/>
-      <c r="V9" s="100" t="s">
+      <c r="V9" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="W9" s="100" t="s">
+      <c r="W9" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="X9" s="100" t="s">
+      <c r="X9" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="Y9" s="100"/>
-      <c r="Z9" s="100"/>
+      <c r="Y9" s="76"/>
+      <c r="Z9" s="76"/>
       <c r="AA9" s="19"/>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.35">
@@ -1947,27 +1968,27 @@
       <c r="I10" s="16"/>
       <c r="J10" s="16"/>
       <c r="K10" s="16"/>
-      <c r="L10" s="100" t="s">
+      <c r="L10" s="76" t="s">
         <v>12</v>
       </c>
       <c r="M10" s="16"/>
       <c r="N10" s="16"/>
       <c r="O10" s="16"/>
       <c r="P10" s="16"/>
-      <c r="Q10" s="100" t="s">
+      <c r="Q10" s="76" t="s">
         <v>11</v>
       </c>
       <c r="R10" s="16"/>
       <c r="S10" s="16"/>
       <c r="T10" s="16"/>
       <c r="U10" s="16"/>
-      <c r="V10" s="100" t="s">
+      <c r="V10" s="76" t="s">
         <v>12</v>
       </c>
       <c r="W10" s="16"/>
       <c r="X10" s="16"/>
-      <c r="Y10" s="100"/>
-      <c r="Z10" s="100"/>
+      <c r="Y10" s="76"/>
+      <c r="Z10" s="76"/>
       <c r="AA10" s="19"/>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.35">
@@ -1990,7 +2011,7 @@
       <c r="I11" s="16"/>
       <c r="J11" s="16"/>
       <c r="K11" s="16"/>
-      <c r="L11" s="103" t="s">
+      <c r="L11" s="79" t="s">
         <v>12</v>
       </c>
       <c r="M11" s="16"/>
@@ -2029,7 +2050,7 @@
       <c r="I12" s="16"/>
       <c r="J12" s="16"/>
       <c r="K12" s="16"/>
-      <c r="L12" s="103" t="s">
+      <c r="L12" s="79" t="s">
         <v>12</v>
       </c>
       <c r="M12" s="16"/>
@@ -2068,7 +2089,7 @@
       <c r="I13" s="16"/>
       <c r="J13" s="16"/>
       <c r="K13" s="16"/>
-      <c r="L13" s="101" t="s">
+      <c r="L13" s="77" t="s">
         <v>11</v>
       </c>
       <c r="M13" s="16"/>
@@ -2107,7 +2128,7 @@
       <c r="I14" s="16"/>
       <c r="J14" s="16"/>
       <c r="K14" s="16"/>
-      <c r="L14" s="101" t="s">
+      <c r="L14" s="77" t="s">
         <v>11</v>
       </c>
       <c r="M14" s="16"/>
@@ -2146,7 +2167,7 @@
       <c r="I15" s="16"/>
       <c r="J15" s="16"/>
       <c r="K15" s="16"/>
-      <c r="L15" s="101" t="s">
+      <c r="L15" s="77" t="s">
         <v>11</v>
       </c>
       <c r="M15" s="16"/>
@@ -2185,8 +2206,8 @@
       </c>
       <c r="H16" s="18"/>
       <c r="I16" s="16"/>
-      <c r="J16" s="102"/>
-      <c r="K16" s="102"/>
+      <c r="J16" s="78"/>
+      <c r="K16" s="78"/>
       <c r="L16" s="16"/>
       <c r="M16" s="16"/>
       <c r="N16" s="16"/>
@@ -2224,8 +2245,8 @@
       </c>
       <c r="H17" s="18"/>
       <c r="I17" s="16"/>
-      <c r="J17" s="102"/>
-      <c r="K17" s="102"/>
+      <c r="J17" s="78"/>
+      <c r="K17" s="78"/>
       <c r="L17" s="16"/>
       <c r="M17" s="16"/>
       <c r="N17" s="16"/>
@@ -2244,10 +2265,10 @@
       <c r="AA17" s="19"/>
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A18" s="105" t="s">
+      <c r="A18" s="81" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="106">
+      <c r="B18" s="82">
         <v>1</v>
       </c>
       <c r="C18" s="37" t="s">
@@ -2263,7 +2284,7 @@
       <c r="I18" s="16"/>
       <c r="J18" s="16"/>
       <c r="K18" s="16"/>
-      <c r="L18" s="104" t="s">
+      <c r="L18" s="80" t="s">
         <v>12</v>
       </c>
       <c r="M18" s="16"/>
@@ -2283,10 +2304,10 @@
       <c r="AA18" s="19"/>
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A19" s="105" t="s">
+      <c r="A19" s="81" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="106">
+      <c r="B19" s="82">
         <v>2</v>
       </c>
       <c r="C19" s="37" t="s">
@@ -2302,10 +2323,10 @@
       <c r="I19" s="16"/>
       <c r="J19" s="16"/>
       <c r="K19" s="16"/>
-      <c r="L19" s="104" t="s">
+      <c r="L19" s="80" t="s">
         <v>12</v>
       </c>
-      <c r="M19" s="104" t="s">
+      <c r="M19" s="80" t="s">
         <v>12</v>
       </c>
       <c r="N19" s="16"/>
@@ -2324,10 +2345,10 @@
       <c r="AA19" s="19"/>
     </row>
     <row r="20" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A20" s="105" t="s">
+      <c r="A20" s="81" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="106">
+      <c r="B20" s="82">
         <v>3</v>
       </c>
       <c r="C20" s="37" t="s">
@@ -2344,10 +2365,10 @@
       <c r="J20" s="16"/>
       <c r="K20" s="16"/>
       <c r="L20" s="16"/>
-      <c r="M20" s="104" t="s">
+      <c r="M20" s="80" t="s">
         <v>12</v>
       </c>
-      <c r="N20" s="104" t="s">
+      <c r="N20" s="80" t="s">
         <v>12</v>
       </c>
       <c r="O20" s="16"/>
@@ -2365,10 +2386,10 @@
       <c r="AA20" s="19"/>
     </row>
     <row r="21" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A21" s="105" t="s">
+      <c r="A21" s="81" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="106">
+      <c r="B21" s="82">
         <v>4</v>
       </c>
       <c r="C21" s="37" t="s">
@@ -2385,13 +2406,13 @@
       <c r="J21" s="16"/>
       <c r="K21" s="16"/>
       <c r="L21" s="16"/>
-      <c r="M21" s="104" t="s">
+      <c r="M21" s="80" t="s">
         <v>12</v>
       </c>
-      <c r="N21" s="104" t="s">
+      <c r="N21" s="80" t="s">
         <v>12</v>
       </c>
-      <c r="O21" s="104" t="s">
+      <c r="O21" s="80" t="s">
         <v>12</v>
       </c>
       <c r="P21" s="16"/>
@@ -2427,7 +2448,7 @@
       <c r="I22" s="16"/>
       <c r="J22" s="16"/>
       <c r="K22" s="16"/>
-      <c r="L22" s="99" t="s">
+      <c r="L22" s="75" t="s">
         <v>12</v>
       </c>
       <c r="M22" s="16"/>
@@ -2466,7 +2487,7 @@
       <c r="I23" s="16"/>
       <c r="J23" s="16"/>
       <c r="K23" s="16"/>
-      <c r="L23" s="99" t="s">
+      <c r="L23" s="75" t="s">
         <v>12</v>
       </c>
       <c r="M23" s="16"/>
@@ -2505,16 +2526,16 @@
       <c r="I24" s="16"/>
       <c r="J24" s="16"/>
       <c r="K24" s="16"/>
-      <c r="L24" s="99" t="s">
+      <c r="L24" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="M24" s="99" t="s">
+      <c r="M24" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="N24" s="99" t="s">
+      <c r="N24" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="O24" s="99" t="s">
+      <c r="O24" s="75" t="s">
         <v>12</v>
       </c>
       <c r="P24" s="16"/>
@@ -2550,7 +2571,7 @@
       <c r="I25" s="16"/>
       <c r="J25" s="16"/>
       <c r="K25" s="16"/>
-      <c r="L25" s="107" t="s">
+      <c r="L25" s="83" t="s">
         <v>10</v>
       </c>
       <c r="M25" s="16"/>
@@ -2589,7 +2610,7 @@
       <c r="I26" s="16"/>
       <c r="J26" s="16"/>
       <c r="K26" s="16"/>
-      <c r="L26" s="107" t="s">
+      <c r="L26" s="83" t="s">
         <v>10</v>
       </c>
       <c r="M26" s="16"/>
@@ -2628,7 +2649,7 @@
       <c r="I27" s="16"/>
       <c r="J27" s="16"/>
       <c r="K27" s="16"/>
-      <c r="L27" s="107" t="s">
+      <c r="L27" s="83" t="s">
         <v>10</v>
       </c>
       <c r="M27" s="16"/>
@@ -2648,10 +2669,10 @@
       <c r="AA27" s="19"/>
     </row>
     <row r="28" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A28" s="108" t="s">
+      <c r="A28" s="84" t="s">
         <v>29</v>
       </c>
-      <c r="B28" s="109">
+      <c r="B28" s="85">
         <v>1</v>
       </c>
       <c r="C28" s="37" t="s">
@@ -2667,13 +2688,13 @@
       <c r="I28" s="16"/>
       <c r="J28" s="16"/>
       <c r="K28" s="16"/>
-      <c r="L28" s="110" t="s">
+      <c r="L28" s="86" t="s">
         <v>11</v>
       </c>
-      <c r="M28" s="110" t="s">
+      <c r="M28" s="86" t="s">
         <v>11</v>
       </c>
-      <c r="N28" s="110" t="s">
+      <c r="N28" s="86" t="s">
         <v>11</v>
       </c>
       <c r="O28" s="16"/>
@@ -2710,10 +2731,10 @@
       <c r="I29" s="16"/>
       <c r="J29" s="16"/>
       <c r="K29" s="16"/>
-      <c r="L29" s="102" t="s">
+      <c r="L29" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="M29" s="102" t="s">
+      <c r="M29" s="78" t="s">
         <v>9</v>
       </c>
       <c r="N29" s="16"/>
@@ -2751,10 +2772,10 @@
       <c r="I30" s="16"/>
       <c r="J30" s="16"/>
       <c r="K30" s="16"/>
-      <c r="L30" s="102" t="s">
+      <c r="L30" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="M30" s="102" t="s">
+      <c r="M30" s="78" t="s">
         <v>9</v>
       </c>
       <c r="N30" s="16"/>
@@ -2794,9 +2815,9 @@
       <c r="I31" s="16"/>
       <c r="J31" s="16"/>
       <c r="K31" s="16"/>
-      <c r="L31" s="111"/>
-      <c r="M31" s="111"/>
-      <c r="N31" s="111"/>
+      <c r="L31" s="87"/>
+      <c r="M31" s="87"/>
+      <c r="N31" s="87"/>
       <c r="O31" s="16"/>
       <c r="P31" s="16"/>
       <c r="Q31" s="16"/>
@@ -2837,18 +2858,18 @@
       <c r="I32" s="16"/>
       <c r="J32" s="16"/>
       <c r="K32" s="16"/>
-      <c r="L32" s="101"/>
-      <c r="M32" s="101"/>
-      <c r="N32" s="101"/>
-      <c r="O32" s="101"/>
-      <c r="P32" s="101"/>
-      <c r="Q32" s="101"/>
-      <c r="R32" s="101"/>
-      <c r="S32" s="101"/>
-      <c r="T32" s="101"/>
-      <c r="U32" s="101"/>
-      <c r="V32" s="101"/>
-      <c r="W32" s="101"/>
+      <c r="L32" s="77"/>
+      <c r="M32" s="77"/>
+      <c r="N32" s="77"/>
+      <c r="O32" s="77"/>
+      <c r="P32" s="77"/>
+      <c r="Q32" s="77"/>
+      <c r="R32" s="77"/>
+      <c r="S32" s="77"/>
+      <c r="T32" s="77"/>
+      <c r="U32" s="77"/>
+      <c r="V32" s="77"/>
+      <c r="W32" s="77"/>
       <c r="X32" s="16"/>
       <c r="Y32" s="16"/>
       <c r="Z32" s="16"/>
@@ -2874,27 +2895,27 @@
       <c r="I33" s="16"/>
       <c r="J33" s="16"/>
       <c r="K33" s="16"/>
-      <c r="L33" s="101" t="s">
+      <c r="L33" s="77" t="s">
         <v>9</v>
       </c>
       <c r="M33" s="16"/>
       <c r="N33" s="16"/>
       <c r="O33" s="16"/>
       <c r="P33" s="16"/>
-      <c r="Q33" s="101" t="s">
+      <c r="Q33" s="77" t="s">
         <v>9</v>
       </c>
       <c r="R33" s="16"/>
       <c r="S33" s="16"/>
       <c r="T33" s="16"/>
       <c r="U33" s="16"/>
-      <c r="V33" s="101" t="s">
+      <c r="V33" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="W33" s="101" t="s">
+      <c r="W33" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="X33" s="101" t="s">
+      <c r="X33" s="77" t="s">
         <v>9</v>
       </c>
       <c r="Y33" s="16"/>
@@ -2959,10 +2980,10 @@
       <c r="J35" s="16"/>
       <c r="K35" s="16"/>
       <c r="L35" s="16"/>
-      <c r="M35" s="112" t="s">
+      <c r="M35" s="88" t="s">
         <v>10</v>
       </c>
-      <c r="N35" s="112" t="s">
+      <c r="N35" s="88" t="s">
         <v>10</v>
       </c>
       <c r="O35" s="16"/>
@@ -3000,10 +3021,10 @@
       <c r="J36" s="16"/>
       <c r="K36" s="16"/>
       <c r="L36" s="16"/>
-      <c r="M36" s="112" t="s">
+      <c r="M36" s="88" t="s">
         <v>10</v>
       </c>
-      <c r="N36" s="112" t="s">
+      <c r="N36" s="88" t="s">
         <v>10</v>
       </c>
       <c r="O36" s="16"/>
@@ -3044,13 +3065,13 @@
       <c r="M37" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="N37" s="112" t="s">
+      <c r="N37" s="88" t="s">
         <v>10</v>
       </c>
-      <c r="O37" s="112" t="s">
+      <c r="O37" s="88" t="s">
         <v>10</v>
       </c>
-      <c r="P37" s="112" t="s">
+      <c r="P37" s="88" t="s">
         <v>10</v>
       </c>
       <c r="Q37" s="16"/>
@@ -3089,16 +3110,16 @@
       <c r="K38" s="16"/>
       <c r="L38" s="16"/>
       <c r="M38" s="16"/>
-      <c r="N38" s="112" t="s">
+      <c r="N38" s="88" t="s">
         <v>10</v>
       </c>
-      <c r="O38" s="112" t="s">
+      <c r="O38" s="88" t="s">
         <v>10</v>
       </c>
-      <c r="P38" s="112" t="s">
+      <c r="P38" s="88" t="s">
         <v>10</v>
       </c>
-      <c r="Q38" s="112" t="s">
+      <c r="Q38" s="88" t="s">
         <v>10</v>
       </c>
       <c r="R38" s="16"/>
@@ -3132,10 +3153,10 @@
       <c r="I39" s="16"/>
       <c r="J39" s="16"/>
       <c r="K39" s="16"/>
-      <c r="L39" s="113" t="s">
+      <c r="L39" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="M39" s="113" t="s">
+      <c r="M39" s="89" t="s">
         <v>9</v>
       </c>
       <c r="N39" s="16"/>
@@ -3173,16 +3194,16 @@
       <c r="I40" s="16"/>
       <c r="J40" s="16"/>
       <c r="K40" s="16"/>
-      <c r="L40" s="113" t="s">
+      <c r="L40" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="M40" s="113" t="s">
+      <c r="M40" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="N40" s="113" t="s">
+      <c r="N40" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="O40" s="113" t="s">
+      <c r="O40" s="89" t="s">
         <v>9</v>
       </c>
       <c r="P40" s="16"/>
@@ -3218,16 +3239,16 @@
       <c r="I41" s="16"/>
       <c r="J41" s="16"/>
       <c r="K41" s="16"/>
-      <c r="L41" s="113" t="s">
+      <c r="L41" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="M41" s="113" t="s">
+      <c r="M41" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="N41" s="113" t="s">
+      <c r="N41" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="O41" s="113" t="s">
+      <c r="O41" s="89" t="s">
         <v>9</v>
       </c>
       <c r="P41" s="16"/>
@@ -3263,22 +3284,22 @@
       <c r="I42" s="16"/>
       <c r="J42" s="16"/>
       <c r="K42" s="16"/>
-      <c r="L42" s="113" t="s">
+      <c r="L42" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="M42" s="113" t="s">
+      <c r="M42" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="N42" s="113" t="s">
+      <c r="N42" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="O42" s="113" t="s">
+      <c r="O42" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="P42" s="113" t="s">
+      <c r="P42" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="Q42" s="113" t="s">
+      <c r="Q42" s="89" t="s">
         <v>9</v>
       </c>
       <c r="R42" s="16"/>
@@ -3315,7 +3336,7 @@
       <c r="L43" s="16"/>
       <c r="M43" s="16"/>
       <c r="N43" s="16"/>
-      <c r="O43" s="115" t="s">
+      <c r="O43" s="91" t="s">
         <v>11</v>
       </c>
       <c r="P43" s="16"/>
@@ -3356,13 +3377,13 @@
       <c r="N44" s="16"/>
       <c r="O44" s="16"/>
       <c r="P44" s="16"/>
-      <c r="Q44" s="102" t="s">
+      <c r="Q44" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="R44" s="102" t="s">
+      <c r="R44" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="S44" s="102" t="s">
+      <c r="S44" s="78" t="s">
         <v>10</v>
       </c>
       <c r="T44" s="16"/>
@@ -3399,13 +3420,13 @@
       <c r="N45" s="16"/>
       <c r="O45" s="16"/>
       <c r="P45" s="16"/>
-      <c r="Q45" s="102" t="s">
+      <c r="Q45" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="R45" s="102" t="s">
+      <c r="R45" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="S45" s="102" t="s">
+      <c r="S45" s="78" t="s">
         <v>9</v>
       </c>
       <c r="T45" s="16"/>
@@ -3444,10 +3465,10 @@
       <c r="N46" s="16"/>
       <c r="O46" s="16"/>
       <c r="P46" s="16"/>
-      <c r="Q46" s="102"/>
-      <c r="R46" s="102"/>
-      <c r="S46" s="102"/>
-      <c r="T46" s="102"/>
+      <c r="Q46" s="78"/>
+      <c r="R46" s="78"/>
+      <c r="S46" s="78"/>
+      <c r="T46" s="78"/>
       <c r="U46" s="16"/>
       <c r="V46" s="16"/>
       <c r="W46" s="16"/>
@@ -3485,16 +3506,16 @@
       <c r="R47" s="16"/>
       <c r="S47" s="16"/>
       <c r="T47" s="16"/>
-      <c r="U47" s="112" t="s">
+      <c r="U47" s="88" t="s">
         <v>9</v>
       </c>
-      <c r="V47" s="112" t="s">
+      <c r="V47" s="88" t="s">
         <v>9</v>
       </c>
-      <c r="W47" s="112" t="s">
+      <c r="W47" s="88" t="s">
         <v>9</v>
       </c>
-      <c r="X47" s="112" t="s">
+      <c r="X47" s="88" t="s">
         <v>9</v>
       </c>
       <c r="Y47" s="16"/>
@@ -3525,23 +3546,23 @@
       </c>
       <c r="H48" s="18"/>
       <c r="I48" s="16"/>
-      <c r="J48" s="98"/>
-      <c r="K48" s="98"/>
-      <c r="L48" s="98"/>
-      <c r="M48" s="98"/>
-      <c r="N48" s="98"/>
-      <c r="O48" s="98"/>
-      <c r="P48" s="98"/>
-      <c r="Q48" s="98"/>
-      <c r="R48" s="98"/>
-      <c r="S48" s="98"/>
-      <c r="T48" s="98"/>
-      <c r="U48" s="98"/>
-      <c r="V48" s="98"/>
-      <c r="W48" s="98"/>
-      <c r="X48" s="98"/>
-      <c r="Y48" s="98"/>
-      <c r="Z48" s="98"/>
+      <c r="J48" s="74"/>
+      <c r="K48" s="74"/>
+      <c r="L48" s="74"/>
+      <c r="M48" s="74"/>
+      <c r="N48" s="74"/>
+      <c r="O48" s="74"/>
+      <c r="P48" s="74"/>
+      <c r="Q48" s="74"/>
+      <c r="R48" s="74"/>
+      <c r="S48" s="74"/>
+      <c r="T48" s="74"/>
+      <c r="U48" s="74"/>
+      <c r="V48" s="74"/>
+      <c r="W48" s="74"/>
+      <c r="X48" s="74"/>
+      <c r="Y48" s="74"/>
+      <c r="Z48" s="74"/>
       <c r="AA48" s="19"/>
     </row>
     <row r="49" spans="1:27" x14ac:dyDescent="0.35">
@@ -3623,12 +3644,12 @@
       <c r="S50" s="16"/>
       <c r="T50" s="16"/>
       <c r="U50" s="16"/>
-      <c r="V50" s="16"/>
-      <c r="W50" s="16"/>
-      <c r="X50" s="16"/>
-      <c r="Y50" s="16"/>
-      <c r="Z50" s="16"/>
-      <c r="AA50" s="19"/>
+      <c r="V50" s="92"/>
+      <c r="W50" s="92"/>
+      <c r="X50" s="92"/>
+      <c r="Y50" s="92"/>
+      <c r="Z50" s="92"/>
+      <c r="AA50" s="93"/>
     </row>
     <row r="51" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A51" s="14" t="s">
@@ -3665,7 +3686,7 @@
       <c r="X51" s="16"/>
       <c r="Y51" s="16"/>
       <c r="Z51" s="16"/>
-      <c r="AA51" s="114" t="s">
+      <c r="AA51" s="90" t="s">
         <v>9</v>
       </c>
     </row>
@@ -3689,8 +3710,12 @@
       <c r="I52" s="1"/>
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
-      <c r="L52" s="1"/>
-      <c r="M52" s="1"/>
+      <c r="L52" s="123" t="s">
+        <v>11</v>
+      </c>
+      <c r="M52" s="123" t="s">
+        <v>11</v>
+      </c>
       <c r="N52" s="1"/>
       <c r="O52" s="1"/>
       <c r="P52" s="1"/>
@@ -3726,8 +3751,12 @@
       <c r="I53" s="1"/>
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
-      <c r="L53" s="1"/>
-      <c r="M53" s="1"/>
+      <c r="L53" s="118" t="s">
+        <v>10</v>
+      </c>
+      <c r="M53" s="118" t="s">
+        <v>10</v>
+      </c>
       <c r="N53" s="1"/>
       <c r="O53" s="1"/>
       <c r="P53" s="1"/>
@@ -3763,8 +3792,12 @@
       <c r="I54" s="1"/>
       <c r="J54" s="1"/>
       <c r="K54" s="1"/>
-      <c r="L54" s="1"/>
-      <c r="M54" s="1"/>
+      <c r="L54" s="124" t="s">
+        <v>10</v>
+      </c>
+      <c r="M54" s="124" t="s">
+        <v>10</v>
+      </c>
       <c r="N54" s="1"/>
       <c r="O54" s="1"/>
       <c r="P54" s="1"/>
@@ -3801,8 +3834,12 @@
       <c r="J55" s="1"/>
       <c r="K55" s="1"/>
       <c r="L55" s="1"/>
-      <c r="M55" s="1"/>
-      <c r="N55" s="1"/>
+      <c r="M55" s="124" t="s">
+        <v>10</v>
+      </c>
+      <c r="N55" s="124" t="s">
+        <v>10</v>
+      </c>
       <c r="O55" s="1"/>
       <c r="P55" s="1"/>
       <c r="Q55" s="1"/>
@@ -3839,14 +3876,22 @@
       <c r="K56" s="1"/>
       <c r="L56" s="1"/>
       <c r="M56" s="1"/>
-      <c r="N56" s="1"/>
-      <c r="O56" s="1"/>
+      <c r="N56" s="124" t="s">
+        <v>10</v>
+      </c>
+      <c r="O56" s="124" t="s">
+        <v>10</v>
+      </c>
       <c r="P56" s="1"/>
       <c r="Q56" s="1"/>
       <c r="R56" s="1"/>
       <c r="S56" s="1"/>
-      <c r="T56" s="1"/>
-      <c r="U56" s="1"/>
+      <c r="T56" s="124" t="s">
+        <v>10</v>
+      </c>
+      <c r="U56" s="124" t="s">
+        <v>10</v>
+      </c>
       <c r="V56" s="1"/>
       <c r="W56" s="1"/>
       <c r="X56" s="1"/>
@@ -3882,9 +3927,15 @@
       <c r="Q57" s="1"/>
       <c r="R57" s="1"/>
       <c r="S57" s="1"/>
-      <c r="T57" s="1"/>
-      <c r="U57" s="1"/>
-      <c r="V57" s="1"/>
+      <c r="T57" s="125" t="s">
+        <v>10</v>
+      </c>
+      <c r="U57" s="125" t="s">
+        <v>10</v>
+      </c>
+      <c r="V57" s="125" t="s">
+        <v>10</v>
+      </c>
       <c r="W57" s="1"/>
       <c r="X57" s="1"/>
       <c r="Y57" s="1"/>
@@ -3911,7 +3962,9 @@
       <c r="I58" s="1"/>
       <c r="J58" s="1"/>
       <c r="K58" s="1"/>
-      <c r="L58" s="1"/>
+      <c r="L58" s="118" t="s">
+        <v>9</v>
+      </c>
       <c r="M58" s="1"/>
       <c r="N58" s="1"/>
       <c r="O58" s="1"/>
@@ -3960,9 +4013,15 @@
       <c r="Q59" s="1"/>
       <c r="R59" s="1"/>
       <c r="S59" s="1"/>
-      <c r="T59" s="1"/>
-      <c r="U59" s="1"/>
-      <c r="V59" s="1"/>
+      <c r="T59" s="118" t="s">
+        <v>9</v>
+      </c>
+      <c r="U59" s="118" t="s">
+        <v>106</v>
+      </c>
+      <c r="V59" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="W59" s="1"/>
       <c r="X59" s="1"/>
       <c r="Y59" s="1"/>
@@ -4001,9 +4060,13 @@
       <c r="Q60" s="1"/>
       <c r="R60" s="1"/>
       <c r="S60" s="1"/>
-      <c r="T60" s="1"/>
-      <c r="U60" s="1"/>
-      <c r="V60" s="1"/>
+      <c r="T60" s="118" t="s">
+        <v>9</v>
+      </c>
+      <c r="U60" s="118" t="s">
+        <v>106</v>
+      </c>
+      <c r="V60" s="118"/>
       <c r="W60" s="1"/>
       <c r="X60" s="1"/>
       <c r="Y60" s="1"/>
@@ -4043,8 +4106,8 @@
       <c r="T61" s="1"/>
       <c r="U61" s="1"/>
       <c r="V61" s="1"/>
-      <c r="W61" s="1"/>
-      <c r="X61" s="1"/>
+      <c r="W61" s="119"/>
+      <c r="X61" s="119"/>
       <c r="Y61" s="1"/>
       <c r="Z61" s="1"/>
       <c r="AA61" s="4"/>
@@ -4083,8 +4146,8 @@
       <c r="U62" s="1"/>
       <c r="V62" s="1"/>
       <c r="W62" s="1"/>
-      <c r="X62" s="1"/>
-      <c r="Y62" s="1"/>
+      <c r="X62" s="120"/>
+      <c r="Y62" s="120"/>
       <c r="Z62" s="1"/>
       <c r="AA62" s="4"/>
     </row>
@@ -4112,20 +4175,20 @@
       <c r="I63" s="1"/>
       <c r="J63" s="1"/>
       <c r="K63" s="1"/>
-      <c r="L63" s="1"/>
-      <c r="M63" s="1"/>
-      <c r="N63" s="1"/>
-      <c r="O63" s="1"/>
-      <c r="P63" s="1"/>
-      <c r="Q63" s="1"/>
-      <c r="R63" s="1"/>
-      <c r="S63" s="1"/>
-      <c r="T63" s="1"/>
-      <c r="U63" s="1"/>
-      <c r="V63" s="1"/>
-      <c r="W63" s="1"/>
-      <c r="X63" s="1"/>
-      <c r="Y63" s="1"/>
+      <c r="L63" s="121"/>
+      <c r="M63" s="121"/>
+      <c r="N63" s="121"/>
+      <c r="O63" s="121"/>
+      <c r="P63" s="121"/>
+      <c r="Q63" s="121"/>
+      <c r="R63" s="121"/>
+      <c r="S63" s="121"/>
+      <c r="T63" s="121"/>
+      <c r="U63" s="121"/>
+      <c r="V63" s="121"/>
+      <c r="W63" s="121"/>
+      <c r="X63" s="121"/>
+      <c r="Y63" s="121"/>
       <c r="Z63" s="1"/>
       <c r="AA63" s="4"/>
     </row>
@@ -4156,28 +4219,28 @@
       <c r="J64" s="1"/>
       <c r="K64" s="1"/>
       <c r="L64" s="1"/>
-      <c r="M64" s="1"/>
-      <c r="N64" s="1"/>
-      <c r="O64" s="1"/>
-      <c r="P64" s="1"/>
-      <c r="Q64" s="1"/>
-      <c r="R64" s="1"/>
-      <c r="S64" s="1"/>
-      <c r="T64" s="1"/>
-      <c r="U64" s="1"/>
-      <c r="V64" s="1"/>
-      <c r="W64" s="1"/>
-      <c r="X64" s="1"/>
-      <c r="Y64" s="1"/>
+      <c r="M64" s="122"/>
+      <c r="N64" s="122"/>
+      <c r="O64" s="122"/>
+      <c r="P64" s="122"/>
+      <c r="Q64" s="122"/>
+      <c r="R64" s="122"/>
+      <c r="S64" s="122"/>
+      <c r="T64" s="122"/>
+      <c r="U64" s="122"/>
+      <c r="V64" s="122"/>
+      <c r="W64" s="122"/>
+      <c r="X64" s="122"/>
+      <c r="Y64" s="122"/>
       <c r="Z64" s="1"/>
       <c r="AA64" s="4"/>
     </row>
     <row r="65" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A65" s="74" t="e">
+      <c r="A65" s="94" t="e">
         <f>+B38:AA68</f>
         <v>#VALUE!</v>
       </c>
-      <c r="B65" s="75"/>
+      <c r="B65" s="95"/>
       <c r="C65" s="38" t="s">
         <v>42</v>
       </c>
@@ -4197,26 +4260,26 @@
         <f>COUNTIF(G5:G64, "X")</f>
         <v>26</v>
       </c>
-      <c r="H65" s="76"/>
-      <c r="I65" s="76"/>
-      <c r="J65" s="76"/>
-      <c r="K65" s="76"/>
-      <c r="L65" s="76"/>
-      <c r="M65" s="76"/>
-      <c r="N65" s="76"/>
-      <c r="O65" s="76"/>
-      <c r="P65" s="76"/>
-      <c r="Q65" s="76"/>
-      <c r="R65" s="76"/>
-      <c r="S65" s="76"/>
-      <c r="T65" s="76"/>
-      <c r="U65" s="76"/>
-      <c r="V65" s="76"/>
-      <c r="W65" s="76"/>
-      <c r="X65" s="76"/>
-      <c r="Y65" s="76"/>
-      <c r="Z65" s="76"/>
-      <c r="AA65" s="77"/>
+      <c r="H65" s="96"/>
+      <c r="I65" s="96"/>
+      <c r="J65" s="96"/>
+      <c r="K65" s="96"/>
+      <c r="L65" s="96"/>
+      <c r="M65" s="96"/>
+      <c r="N65" s="96"/>
+      <c r="O65" s="96"/>
+      <c r="P65" s="96"/>
+      <c r="Q65" s="96"/>
+      <c r="R65" s="96"/>
+      <c r="S65" s="96"/>
+      <c r="T65" s="96"/>
+      <c r="U65" s="96"/>
+      <c r="V65" s="96"/>
+      <c r="W65" s="96"/>
+      <c r="X65" s="96"/>
+      <c r="Y65" s="96"/>
+      <c r="Z65" s="96"/>
+      <c r="AA65" s="97"/>
     </row>
     <row r="66" spans="1:27" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>

</xml_diff>

<commit_message>
Set of characters in space, read description
-Created a set of characters in space
-Implemented it in space
-Fixed functions that used the old functions
-Fixed attack so it uses an argument
-Fixed chat so it uses an argument
-Updated excel
</commit_message>
<xml_diff>
--- a/Reuniones_Coordinacion/Diagrama_Gantt_8_4_25_Saul_Fernando_Raquel_Irene.xlsx
+++ b/Reuniones_Coordinacion/Diagrama_Gantt_8_4_25_Saul_Fernando_Raquel_Irene.xlsx
@@ -5,21 +5,31 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\saul\Pprog_conversation\Reuniones_Coordinacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\fernandpo\cosa_uni\proyecto_program\Reuniones_Coordinacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF80DCE8-2C5E-4460-8663-8EED5EDADDCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C79EA513-F26B-4A97-8823-4751DF0038F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{76F30C29-DD84-4491-9B4C-00A38B383DA8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{76F30C29-DD84-4491-9B4C-00A38B383DA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -184,9 +194,6 @@
     <t>Game_actions: modificar move (seguidores)</t>
   </si>
   <si>
-    <t>Game_actions: modificar chat</t>
-  </si>
-  <si>
     <t>Game_actions: modificar move (up/down)</t>
   </si>
   <si>
@@ -347,13 +354,16 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Game_actions: modificar chat y attack</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -361,8 +371,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="26">
+  <fills count="27">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -513,6 +531,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="31">
     <border>
@@ -950,7 +974,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="130">
+  <cellXfs count="132">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1179,78 +1203,6 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1279,6 +1231,84 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1362,9 +1392,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1402,7 +1432,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1508,7 +1538,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1650,7 +1680,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1660,130 +1690,130 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13B8C02F-838E-4995-8CF9-185661B72170}">
   <dimension ref="A1:AA66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C58" zoomScale="115" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="135" zoomScaleNormal="135" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="3.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="3.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="24" width="3" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="2.90625" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="2.88671875" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="94" t="s">
+    <row r="1" spans="1:27" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="110" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="95"/>
-      <c r="C1" s="95"/>
-      <c r="D1" s="95"/>
-      <c r="E1" s="95"/>
-      <c r="F1" s="95"/>
-      <c r="G1" s="95"/>
-      <c r="H1" s="95"/>
-      <c r="I1" s="95"/>
-      <c r="J1" s="95"/>
-      <c r="K1" s="95"/>
-      <c r="L1" s="95"/>
-      <c r="M1" s="95"/>
-      <c r="N1" s="95"/>
-      <c r="O1" s="95"/>
-      <c r="P1" s="95"/>
-      <c r="Q1" s="95"/>
-      <c r="R1" s="95"/>
-      <c r="S1" s="95"/>
-      <c r="T1" s="95"/>
-      <c r="U1" s="95"/>
-      <c r="V1" s="95"/>
-      <c r="W1" s="95"/>
-      <c r="X1" s="95"/>
-      <c r="Y1" s="95"/>
-      <c r="Z1" s="95"/>
-      <c r="AA1" s="96"/>
-    </row>
-    <row r="2" spans="1:27" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="97" t="s">
+      <c r="B1" s="111"/>
+      <c r="C1" s="111"/>
+      <c r="D1" s="111"/>
+      <c r="E1" s="111"/>
+      <c r="F1" s="111"/>
+      <c r="G1" s="111"/>
+      <c r="H1" s="111"/>
+      <c r="I1" s="111"/>
+      <c r="J1" s="111"/>
+      <c r="K1" s="111"/>
+      <c r="L1" s="111"/>
+      <c r="M1" s="111"/>
+      <c r="N1" s="111"/>
+      <c r="O1" s="111"/>
+      <c r="P1" s="111"/>
+      <c r="Q1" s="111"/>
+      <c r="R1" s="111"/>
+      <c r="S1" s="111"/>
+      <c r="T1" s="111"/>
+      <c r="U1" s="111"/>
+      <c r="V1" s="111"/>
+      <c r="W1" s="111"/>
+      <c r="X1" s="111"/>
+      <c r="Y1" s="111"/>
+      <c r="Z1" s="111"/>
+      <c r="AA1" s="112"/>
+    </row>
+    <row r="2" spans="1:27" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="113" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="98"/>
-      <c r="C2" s="103" t="s">
+      <c r="B2" s="114"/>
+      <c r="C2" s="119" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="106" t="s">
+      <c r="D2" s="122" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="106"/>
-      <c r="F2" s="106"/>
-      <c r="G2" s="107"/>
-      <c r="H2" s="110" t="s">
+      <c r="E2" s="122"/>
+      <c r="F2" s="122"/>
+      <c r="G2" s="123"/>
+      <c r="H2" s="126" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="106"/>
-      <c r="J2" s="106"/>
-      <c r="K2" s="106"/>
-      <c r="L2" s="106"/>
-      <c r="M2" s="106"/>
-      <c r="N2" s="106"/>
-      <c r="O2" s="106"/>
-      <c r="P2" s="106"/>
-      <c r="Q2" s="106"/>
-      <c r="R2" s="106"/>
-      <c r="S2" s="106"/>
-      <c r="T2" s="106"/>
-      <c r="U2" s="106"/>
-      <c r="V2" s="106"/>
-      <c r="W2" s="106"/>
-      <c r="X2" s="106"/>
-      <c r="Y2" s="106"/>
-      <c r="Z2" s="106"/>
-      <c r="AA2" s="111"/>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A3" s="99"/>
-      <c r="B3" s="100"/>
-      <c r="C3" s="104"/>
-      <c r="D3" s="108"/>
-      <c r="E3" s="108"/>
-      <c r="F3" s="108"/>
-      <c r="G3" s="109"/>
-      <c r="H3" s="112" t="s">
+      <c r="I2" s="122"/>
+      <c r="J2" s="122"/>
+      <c r="K2" s="122"/>
+      <c r="L2" s="122"/>
+      <c r="M2" s="122"/>
+      <c r="N2" s="122"/>
+      <c r="O2" s="122"/>
+      <c r="P2" s="122"/>
+      <c r="Q2" s="122"/>
+      <c r="R2" s="122"/>
+      <c r="S2" s="122"/>
+      <c r="T2" s="122"/>
+      <c r="U2" s="122"/>
+      <c r="V2" s="122"/>
+      <c r="W2" s="122"/>
+      <c r="X2" s="122"/>
+      <c r="Y2" s="122"/>
+      <c r="Z2" s="122"/>
+      <c r="AA2" s="127"/>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A3" s="115"/>
+      <c r="B3" s="116"/>
+      <c r="C3" s="120"/>
+      <c r="D3" s="124"/>
+      <c r="E3" s="124"/>
+      <c r="F3" s="124"/>
+      <c r="G3" s="125"/>
+      <c r="H3" s="128" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="108"/>
-      <c r="J3" s="108"/>
-      <c r="K3" s="108"/>
-      <c r="L3" s="108"/>
-      <c r="M3" s="108" t="s">
+      <c r="I3" s="124"/>
+      <c r="J3" s="124"/>
+      <c r="K3" s="124"/>
+      <c r="L3" s="124"/>
+      <c r="M3" s="124" t="s">
         <v>6</v>
       </c>
-      <c r="N3" s="108"/>
-      <c r="O3" s="108"/>
-      <c r="P3" s="108"/>
-      <c r="Q3" s="108"/>
-      <c r="R3" s="108" t="s">
+      <c r="N3" s="124"/>
+      <c r="O3" s="124"/>
+      <c r="P3" s="124"/>
+      <c r="Q3" s="124"/>
+      <c r="R3" s="124" t="s">
         <v>7</v>
       </c>
-      <c r="S3" s="108"/>
-      <c r="T3" s="108"/>
-      <c r="U3" s="108"/>
-      <c r="V3" s="108"/>
-      <c r="W3" s="108" t="s">
+      <c r="S3" s="124"/>
+      <c r="T3" s="124"/>
+      <c r="U3" s="124"/>
+      <c r="V3" s="124"/>
+      <c r="W3" s="124" t="s">
         <v>8</v>
       </c>
-      <c r="X3" s="108"/>
-      <c r="Y3" s="108"/>
-      <c r="Z3" s="108"/>
-      <c r="AA3" s="113"/>
-    </row>
-    <row r="4" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="101"/>
-      <c r="B4" s="102"/>
-      <c r="C4" s="105"/>
+      <c r="X3" s="124"/>
+      <c r="Y3" s="124"/>
+      <c r="Z3" s="124"/>
+      <c r="AA3" s="129"/>
+    </row>
+    <row r="4" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="117"/>
+      <c r="B4" s="118"/>
+      <c r="C4" s="121"/>
       <c r="D4" s="66" t="s">
         <v>9</v>
       </c>
@@ -1857,7 +1887,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:27" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A5" s="59" t="s">
         <v>13</v>
       </c>
@@ -1879,8 +1909,8 @@
       <c r="G5" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="122"/>
-      <c r="I5" s="123"/>
+      <c r="H5" s="98"/>
+      <c r="I5" s="99"/>
       <c r="J5" s="62"/>
       <c r="K5" s="64"/>
       <c r="L5" s="62"/>
@@ -1900,7 +1930,7 @@
       <c r="Z5" s="64"/>
       <c r="AA5" s="65"/>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
@@ -1918,8 +1948,8 @@
       <c r="G6" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="124"/>
-      <c r="I6" s="125"/>
+      <c r="H6" s="100"/>
+      <c r="I6" s="101"/>
       <c r="J6" s="15"/>
       <c r="K6" s="15"/>
       <c r="L6" s="71"/>
@@ -1939,7 +1969,7 @@
       <c r="Z6" s="71"/>
       <c r="AA6" s="17"/>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
@@ -1961,8 +1991,8 @@
       <c r="G7" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="124"/>
-      <c r="I7" s="125"/>
+      <c r="H7" s="100"/>
+      <c r="I7" s="101"/>
       <c r="J7" s="15"/>
       <c r="K7" s="15"/>
       <c r="L7" s="71"/>
@@ -1982,7 +2012,7 @@
       <c r="Z7" s="71"/>
       <c r="AA7" s="17"/>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
@@ -2004,8 +2034,8 @@
       <c r="G8" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="124"/>
-      <c r="I8" s="125"/>
+      <c r="H8" s="100"/>
+      <c r="I8" s="101"/>
       <c r="J8" s="15"/>
       <c r="K8" s="15"/>
       <c r="L8" s="71"/>
@@ -2025,7 +2055,7 @@
       <c r="Z8" s="71"/>
       <c r="AA8" s="17"/>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>20</v>
       </c>
@@ -2045,8 +2075,8 @@
       <c r="G9" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="H9" s="124"/>
-      <c r="I9" s="125"/>
+      <c r="H9" s="100"/>
+      <c r="I9" s="101"/>
       <c r="J9" s="15"/>
       <c r="K9" s="15"/>
       <c r="L9" s="72" t="s">
@@ -2076,7 +2106,7 @@
       <c r="Z9" s="72"/>
       <c r="AA9" s="17"/>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>20</v>
       </c>
@@ -2094,8 +2124,8 @@
       <c r="G10" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="H10" s="124"/>
-      <c r="I10" s="125"/>
+      <c r="H10" s="100"/>
+      <c r="I10" s="101"/>
       <c r="J10" s="15"/>
       <c r="K10" s="15"/>
       <c r="L10" s="72" t="s">
@@ -2121,7 +2151,7 @@
       <c r="Z10" s="72"/>
       <c r="AA10" s="17"/>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>23</v>
       </c>
@@ -2137,8 +2167,8 @@
       <c r="G11" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="H11" s="124"/>
-      <c r="I11" s="125"/>
+      <c r="H11" s="100"/>
+      <c r="I11" s="101"/>
       <c r="J11" s="15"/>
       <c r="K11" s="15"/>
       <c r="L11" s="75" t="s">
@@ -2160,7 +2190,7 @@
       <c r="Z11" s="15"/>
       <c r="AA11" s="17"/>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>23</v>
       </c>
@@ -2176,8 +2206,8 @@
       <c r="G12" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="H12" s="124"/>
-      <c r="I12" s="125"/>
+      <c r="H12" s="100"/>
+      <c r="I12" s="101"/>
       <c r="J12" s="15"/>
       <c r="K12" s="15"/>
       <c r="L12" s="75" t="s">
@@ -2199,7 +2229,7 @@
       <c r="Z12" s="15"/>
       <c r="AA12" s="17"/>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A13" s="18" t="s">
         <v>24</v>
       </c>
@@ -2215,8 +2245,8 @@
         <v>15</v>
       </c>
       <c r="G13" s="16"/>
-      <c r="H13" s="124"/>
-      <c r="I13" s="125"/>
+      <c r="H13" s="100"/>
+      <c r="I13" s="101"/>
       <c r="J13" s="15"/>
       <c r="K13" s="15"/>
       <c r="L13" s="73" t="s">
@@ -2238,7 +2268,7 @@
       <c r="Z13" s="15"/>
       <c r="AA13" s="17"/>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
         <v>24</v>
       </c>
@@ -2254,8 +2284,8 @@
         <v>15</v>
       </c>
       <c r="G14" s="16"/>
-      <c r="H14" s="124"/>
-      <c r="I14" s="125"/>
+      <c r="H14" s="100"/>
+      <c r="I14" s="101"/>
       <c r="J14" s="15"/>
       <c r="K14" s="15"/>
       <c r="L14" s="73" t="s">
@@ -2277,7 +2307,7 @@
       <c r="Z14" s="15"/>
       <c r="AA14" s="17"/>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A15" s="18" t="s">
         <v>24</v>
       </c>
@@ -2293,8 +2323,8 @@
         <v>15</v>
       </c>
       <c r="G15" s="16"/>
-      <c r="H15" s="124"/>
-      <c r="I15" s="125"/>
+      <c r="H15" s="100"/>
+      <c r="I15" s="101"/>
       <c r="J15" s="15"/>
       <c r="K15" s="15"/>
       <c r="L15" s="73" t="s">
@@ -2316,7 +2346,7 @@
       <c r="Z15" s="15"/>
       <c r="AA15" s="17"/>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A16" s="19" t="s">
         <v>25</v>
       </c>
@@ -2334,8 +2364,8 @@
       <c r="G16" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="H16" s="124"/>
-      <c r="I16" s="125"/>
+      <c r="H16" s="100"/>
+      <c r="I16" s="101"/>
       <c r="J16" s="74"/>
       <c r="K16" s="74"/>
       <c r="L16" s="15"/>
@@ -2355,7 +2385,7 @@
       <c r="Z16" s="15"/>
       <c r="AA16" s="17"/>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A17" s="19" t="s">
         <v>25</v>
       </c>
@@ -2373,8 +2403,8 @@
       <c r="G17" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="H17" s="124"/>
-      <c r="I17" s="125"/>
+      <c r="H17" s="100"/>
+      <c r="I17" s="101"/>
       <c r="J17" s="74"/>
       <c r="K17" s="74"/>
       <c r="L17" s="15"/>
@@ -2394,7 +2424,7 @@
       <c r="Z17" s="15"/>
       <c r="AA17" s="17"/>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A18" s="77" t="s">
         <v>26</v>
       </c>
@@ -2407,11 +2437,11 @@
       <c r="D18" s="15"/>
       <c r="E18" s="15"/>
       <c r="F18" s="15"/>
-      <c r="G18" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="H18" s="124"/>
-      <c r="I18" s="125"/>
+      <c r="G18" s="130" t="s">
+        <v>15</v>
+      </c>
+      <c r="H18" s="100"/>
+      <c r="I18" s="101"/>
       <c r="J18" s="15"/>
       <c r="K18" s="15"/>
       <c r="L18" s="76" t="s">
@@ -2433,7 +2463,7 @@
       <c r="Z18" s="15"/>
       <c r="AA18" s="17"/>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A19" s="77" t="s">
         <v>26</v>
       </c>
@@ -2449,8 +2479,8 @@
       <c r="G19" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="H19" s="124"/>
-      <c r="I19" s="125"/>
+      <c r="H19" s="100"/>
+      <c r="I19" s="101"/>
       <c r="J19" s="15"/>
       <c r="K19" s="15"/>
       <c r="L19" s="76" t="s">
@@ -2474,7 +2504,7 @@
       <c r="Z19" s="15"/>
       <c r="AA19" s="17"/>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A20" s="77" t="s">
         <v>26</v>
       </c>
@@ -2482,16 +2512,16 @@
         <v>3</v>
       </c>
       <c r="C20" s="34" t="s">
-        <v>52</v>
+        <v>106</v>
       </c>
       <c r="D20" s="15"/>
       <c r="E20" s="15"/>
       <c r="F20" s="15"/>
-      <c r="G20" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="H20" s="124"/>
-      <c r="I20" s="125"/>
+      <c r="G20" s="131" t="s">
+        <v>15</v>
+      </c>
+      <c r="H20" s="100"/>
+      <c r="I20" s="101"/>
       <c r="J20" s="15"/>
       <c r="K20" s="15"/>
       <c r="L20" s="15"/>
@@ -2515,7 +2545,7 @@
       <c r="Z20" s="15"/>
       <c r="AA20" s="17"/>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A21" s="77" t="s">
         <v>26</v>
       </c>
@@ -2523,7 +2553,7 @@
         <v>4</v>
       </c>
       <c r="C21" s="34" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D21" s="15"/>
       <c r="E21" s="15"/>
@@ -2531,8 +2561,8 @@
       <c r="G21" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="H21" s="124"/>
-      <c r="I21" s="125"/>
+      <c r="H21" s="100"/>
+      <c r="I21" s="101"/>
       <c r="J21" s="15"/>
       <c r="K21" s="15"/>
       <c r="L21" s="15"/>
@@ -2558,7 +2588,7 @@
       <c r="Z21" s="15"/>
       <c r="AA21" s="17"/>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>27</v>
       </c>
@@ -2566,7 +2596,7 @@
         <v>1</v>
       </c>
       <c r="C22" s="34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D22" s="15"/>
       <c r="E22" s="15"/>
@@ -2574,8 +2604,8 @@
       <c r="G22" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="H22" s="124"/>
-      <c r="I22" s="125"/>
+      <c r="H22" s="100"/>
+      <c r="I22" s="101"/>
       <c r="J22" s="15"/>
       <c r="K22" s="15"/>
       <c r="L22" s="71" t="s">
@@ -2597,7 +2627,7 @@
       <c r="Z22" s="15"/>
       <c r="AA22" s="17"/>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>27</v>
       </c>
@@ -2605,7 +2635,7 @@
         <v>2</v>
       </c>
       <c r="C23" s="34" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D23" s="15"/>
       <c r="E23" s="15"/>
@@ -2613,8 +2643,8 @@
       <c r="G23" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="H23" s="124"/>
-      <c r="I23" s="125"/>
+      <c r="H23" s="100"/>
+      <c r="I23" s="101"/>
       <c r="J23" s="15"/>
       <c r="K23" s="15"/>
       <c r="L23" s="71" t="s">
@@ -2636,7 +2666,7 @@
       <c r="Z23" s="15"/>
       <c r="AA23" s="17"/>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>27</v>
       </c>
@@ -2644,7 +2674,7 @@
         <v>3</v>
       </c>
       <c r="C24" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D24" s="15"/>
       <c r="E24" s="15"/>
@@ -2652,8 +2682,8 @@
       <c r="G24" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="H24" s="124"/>
-      <c r="I24" s="125"/>
+      <c r="H24" s="100"/>
+      <c r="I24" s="101"/>
       <c r="J24" s="15"/>
       <c r="K24" s="15"/>
       <c r="L24" s="71" t="s">
@@ -2681,7 +2711,7 @@
       <c r="Z24" s="15"/>
       <c r="AA24" s="17"/>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
         <v>28</v>
       </c>
@@ -2689,7 +2719,7 @@
         <v>1</v>
       </c>
       <c r="C25" s="34" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D25" s="15"/>
       <c r="E25" s="15" t="s">
@@ -2697,8 +2727,8 @@
       </c>
       <c r="F25" s="15"/>
       <c r="G25" s="16"/>
-      <c r="H25" s="124"/>
-      <c r="I25" s="125"/>
+      <c r="H25" s="100"/>
+      <c r="I25" s="101"/>
       <c r="J25" s="15"/>
       <c r="K25" s="15"/>
       <c r="L25" s="79" t="s">
@@ -2720,7 +2750,7 @@
       <c r="Z25" s="15"/>
       <c r="AA25" s="17"/>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
         <v>28</v>
       </c>
@@ -2728,7 +2758,7 @@
         <v>2</v>
       </c>
       <c r="C26" s="34" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D26" s="15"/>
       <c r="E26" s="15" t="s">
@@ -2736,8 +2766,8 @@
       </c>
       <c r="F26" s="15"/>
       <c r="G26" s="16"/>
-      <c r="H26" s="124"/>
-      <c r="I26" s="125"/>
+      <c r="H26" s="100"/>
+      <c r="I26" s="101"/>
       <c r="J26" s="15"/>
       <c r="K26" s="15"/>
       <c r="L26" s="79" t="s">
@@ -2759,7 +2789,7 @@
       <c r="Z26" s="15"/>
       <c r="AA26" s="17"/>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
         <v>28</v>
       </c>
@@ -2767,7 +2797,7 @@
         <v>3</v>
       </c>
       <c r="C27" s="34" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D27" s="15"/>
       <c r="E27" s="15" t="s">
@@ -2775,8 +2805,8 @@
       </c>
       <c r="F27" s="15"/>
       <c r="G27" s="16"/>
-      <c r="H27" s="124"/>
-      <c r="I27" s="125"/>
+      <c r="H27" s="100"/>
+      <c r="I27" s="101"/>
       <c r="J27" s="15"/>
       <c r="K27" s="15"/>
       <c r="L27" s="79" t="s">
@@ -2798,7 +2828,7 @@
       <c r="Z27" s="15"/>
       <c r="AA27" s="17"/>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A28" s="80" t="s">
         <v>29</v>
       </c>
@@ -2806,7 +2836,7 @@
         <v>1</v>
       </c>
       <c r="C28" s="34" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D28" s="15"/>
       <c r="E28" s="15"/>
@@ -2814,8 +2844,8 @@
         <v>15</v>
       </c>
       <c r="G28" s="16"/>
-      <c r="H28" s="124"/>
-      <c r="I28" s="125"/>
+      <c r="H28" s="100"/>
+      <c r="I28" s="101"/>
       <c r="J28" s="15"/>
       <c r="K28" s="15"/>
       <c r="L28" s="82" t="s">
@@ -2841,7 +2871,7 @@
       <c r="Z28" s="15"/>
       <c r="AA28" s="17"/>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
         <v>30</v>
       </c>
@@ -2849,7 +2879,7 @@
         <v>1</v>
       </c>
       <c r="C29" s="34" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D29" s="15" t="s">
         <v>15</v>
@@ -2857,8 +2887,8 @@
       <c r="E29" s="15"/>
       <c r="F29" s="15"/>
       <c r="G29" s="16"/>
-      <c r="H29" s="124"/>
-      <c r="I29" s="125"/>
+      <c r="H29" s="100"/>
+      <c r="I29" s="101"/>
       <c r="J29" s="15"/>
       <c r="K29" s="15"/>
       <c r="L29" s="74" t="s">
@@ -2882,7 +2912,7 @@
       <c r="Z29" s="15"/>
       <c r="AA29" s="17"/>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
         <v>30</v>
       </c>
@@ -2890,7 +2920,7 @@
         <v>2</v>
       </c>
       <c r="C30" s="34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D30" s="15" t="s">
         <v>15</v>
@@ -2898,8 +2928,8 @@
       <c r="E30" s="15"/>
       <c r="F30" s="15"/>
       <c r="G30" s="16"/>
-      <c r="H30" s="124"/>
-      <c r="I30" s="125"/>
+      <c r="H30" s="100"/>
+      <c r="I30" s="101"/>
       <c r="J30" s="15"/>
       <c r="K30" s="15"/>
       <c r="L30" s="74" t="s">
@@ -2923,7 +2953,7 @@
       <c r="Z30" s="15"/>
       <c r="AA30" s="17"/>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A31" s="8" t="s">
         <v>31</v>
       </c>
@@ -2931,7 +2961,7 @@
         <v>1</v>
       </c>
       <c r="C31" s="34" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D31" s="15"/>
       <c r="E31" s="15"/>
@@ -2941,8 +2971,8 @@
       <c r="G31" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="H31" s="124"/>
-      <c r="I31" s="125"/>
+      <c r="H31" s="100"/>
+      <c r="I31" s="101"/>
       <c r="J31" s="15"/>
       <c r="K31" s="15"/>
       <c r="L31" s="83"/>
@@ -2962,7 +2992,7 @@
       <c r="Z31" s="15"/>
       <c r="AA31" s="17"/>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A32" s="18" t="s">
         <v>32</v>
       </c>
@@ -2970,7 +3000,7 @@
         <v>1</v>
       </c>
       <c r="C32" s="34" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D32" s="15" t="s">
         <v>15</v>
@@ -2984,8 +3014,8 @@
       <c r="G32" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="H32" s="124"/>
-      <c r="I32" s="125"/>
+      <c r="H32" s="100"/>
+      <c r="I32" s="101"/>
       <c r="J32" s="15"/>
       <c r="K32" s="15"/>
       <c r="L32" s="73"/>
@@ -3005,7 +3035,7 @@
       <c r="Z32" s="15"/>
       <c r="AA32" s="17"/>
     </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A33" s="18" t="s">
         <v>32</v>
       </c>
@@ -3013,7 +3043,7 @@
         <v>2</v>
       </c>
       <c r="C33" s="34" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D33" s="15" t="s">
         <v>15</v>
@@ -3021,8 +3051,8 @@
       <c r="E33" s="15"/>
       <c r="F33" s="15"/>
       <c r="G33" s="16"/>
-      <c r="H33" s="124"/>
-      <c r="I33" s="125"/>
+      <c r="H33" s="100"/>
+      <c r="I33" s="101"/>
       <c r="J33" s="15"/>
       <c r="K33" s="15"/>
       <c r="L33" s="73" t="s">
@@ -3052,7 +3082,7 @@
       <c r="Z33" s="15"/>
       <c r="AA33" s="17"/>
     </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="s">
         <v>33</v>
       </c>
@@ -3060,7 +3090,7 @@
         <v>1</v>
       </c>
       <c r="C34" s="34" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D34" s="15"/>
       <c r="E34" s="15" t="s">
@@ -3068,8 +3098,8 @@
       </c>
       <c r="F34" s="15"/>
       <c r="G34" s="16"/>
-      <c r="H34" s="124"/>
-      <c r="I34" s="125"/>
+      <c r="H34" s="100"/>
+      <c r="I34" s="101"/>
       <c r="J34" s="15"/>
       <c r="K34" s="15"/>
       <c r="L34" s="15"/>
@@ -3089,7 +3119,7 @@
       <c r="Z34" s="15"/>
       <c r="AA34" s="17"/>
     </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A35" s="10" t="s">
         <v>33</v>
       </c>
@@ -3097,7 +3127,7 @@
         <v>2</v>
       </c>
       <c r="C35" s="34" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D35" s="15"/>
       <c r="E35" s="15" t="s">
@@ -3105,8 +3135,8 @@
       </c>
       <c r="F35" s="15"/>
       <c r="G35" s="16"/>
-      <c r="H35" s="124"/>
-      <c r="I35" s="125"/>
+      <c r="H35" s="100"/>
+      <c r="I35" s="101"/>
       <c r="J35" s="15"/>
       <c r="K35" s="15"/>
       <c r="L35" s="15"/>
@@ -3130,7 +3160,7 @@
       <c r="Z35" s="15"/>
       <c r="AA35" s="17"/>
     </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A36" s="10" t="s">
         <v>33</v>
       </c>
@@ -3138,7 +3168,7 @@
         <v>3</v>
       </c>
       <c r="C36" s="34" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D36" s="15"/>
       <c r="E36" s="15" t="s">
@@ -3146,8 +3176,8 @@
       </c>
       <c r="F36" s="15"/>
       <c r="G36" s="16"/>
-      <c r="H36" s="124"/>
-      <c r="I36" s="125"/>
+      <c r="H36" s="100"/>
+      <c r="I36" s="101"/>
       <c r="J36" s="15"/>
       <c r="K36" s="15"/>
       <c r="L36" s="15"/>
@@ -3171,7 +3201,7 @@
       <c r="Z36" s="15"/>
       <c r="AA36" s="17"/>
     </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A37" s="10" t="s">
         <v>33</v>
       </c>
@@ -3179,7 +3209,7 @@
         <v>4</v>
       </c>
       <c r="C37" s="34" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D37" s="15"/>
       <c r="E37" s="15" t="s">
@@ -3187,13 +3217,13 @@
       </c>
       <c r="F37" s="15"/>
       <c r="G37" s="16"/>
-      <c r="H37" s="124"/>
-      <c r="I37" s="125"/>
+      <c r="H37" s="100"/>
+      <c r="I37" s="101"/>
       <c r="J37" s="15"/>
       <c r="K37" s="15"/>
       <c r="L37" s="15"/>
       <c r="M37" s="15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="N37" s="84" t="s">
         <v>10</v>
@@ -3216,7 +3246,7 @@
       <c r="Z37" s="15"/>
       <c r="AA37" s="17"/>
     </row>
-    <row r="38" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A38" s="10" t="s">
         <v>33</v>
       </c>
@@ -3224,7 +3254,7 @@
         <v>5</v>
       </c>
       <c r="C38" s="34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D38" s="15" t="s">
         <v>15</v>
@@ -3234,8 +3264,8 @@
       </c>
       <c r="F38" s="15"/>
       <c r="G38" s="16"/>
-      <c r="H38" s="124"/>
-      <c r="I38" s="125"/>
+      <c r="H38" s="100"/>
+      <c r="I38" s="101"/>
       <c r="J38" s="15"/>
       <c r="K38" s="15"/>
       <c r="L38" s="15"/>
@@ -3263,7 +3293,7 @@
       <c r="Z38" s="15"/>
       <c r="AA38" s="17"/>
     </row>
-    <row r="39" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A39" s="9" t="s">
         <v>34</v>
       </c>
@@ -3271,7 +3301,7 @@
         <v>1</v>
       </c>
       <c r="C39" s="34" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D39" s="15" t="s">
         <v>15</v>
@@ -3279,8 +3309,8 @@
       <c r="E39" s="15"/>
       <c r="F39" s="15"/>
       <c r="G39" s="16"/>
-      <c r="H39" s="124"/>
-      <c r="I39" s="125"/>
+      <c r="H39" s="100"/>
+      <c r="I39" s="101"/>
       <c r="J39" s="15"/>
       <c r="K39" s="15"/>
       <c r="L39" s="85" t="s">
@@ -3304,7 +3334,7 @@
       <c r="Z39" s="15"/>
       <c r="AA39" s="17"/>
     </row>
-    <row r="40" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A40" s="9" t="s">
         <v>34</v>
       </c>
@@ -3312,7 +3342,7 @@
         <v>2</v>
       </c>
       <c r="C40" s="34" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D40" s="15" t="s">
         <v>15</v>
@@ -3320,8 +3350,8 @@
       <c r="E40" s="15"/>
       <c r="F40" s="15"/>
       <c r="G40" s="16"/>
-      <c r="H40" s="124"/>
-      <c r="I40" s="125"/>
+      <c r="H40" s="100"/>
+      <c r="I40" s="101"/>
       <c r="J40" s="15"/>
       <c r="K40" s="15"/>
       <c r="L40" s="85" t="s">
@@ -3349,7 +3379,7 @@
       <c r="Z40" s="15"/>
       <c r="AA40" s="17"/>
     </row>
-    <row r="41" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A41" s="9" t="s">
         <v>34</v>
       </c>
@@ -3357,7 +3387,7 @@
         <v>3</v>
       </c>
       <c r="C41" s="34" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D41" s="15" t="s">
         <v>15</v>
@@ -3365,8 +3395,8 @@
       <c r="E41" s="15"/>
       <c r="F41" s="15"/>
       <c r="G41" s="16"/>
-      <c r="H41" s="124"/>
-      <c r="I41" s="125"/>
+      <c r="H41" s="100"/>
+      <c r="I41" s="101"/>
       <c r="J41" s="15"/>
       <c r="K41" s="15"/>
       <c r="L41" s="85" t="s">
@@ -3394,7 +3424,7 @@
       <c r="Z41" s="15"/>
       <c r="AA41" s="17"/>
     </row>
-    <row r="42" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A42" s="9" t="s">
         <v>34</v>
       </c>
@@ -3402,7 +3432,7 @@
         <v>4</v>
       </c>
       <c r="C42" s="34" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D42" s="15" t="s">
         <v>15</v>
@@ -3410,8 +3440,8 @@
       <c r="E42" s="15"/>
       <c r="F42" s="15"/>
       <c r="G42" s="16"/>
-      <c r="H42" s="124"/>
-      <c r="I42" s="125"/>
+      <c r="H42" s="100"/>
+      <c r="I42" s="101"/>
       <c r="J42" s="15"/>
       <c r="K42" s="15"/>
       <c r="L42" s="85" t="s">
@@ -3443,7 +3473,7 @@
       <c r="Z42" s="15"/>
       <c r="AA42" s="17"/>
     </row>
-    <row r="43" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A43" s="20" t="s">
         <v>36</v>
       </c>
@@ -3451,7 +3481,7 @@
         <v>1</v>
       </c>
       <c r="C43" s="34" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D43" s="15"/>
       <c r="E43" s="15"/>
@@ -3459,8 +3489,8 @@
         <v>15</v>
       </c>
       <c r="G43" s="16"/>
-      <c r="H43" s="124"/>
-      <c r="I43" s="125"/>
+      <c r="H43" s="100"/>
+      <c r="I43" s="101"/>
       <c r="J43" s="15"/>
       <c r="K43" s="15"/>
       <c r="L43" s="15"/>
@@ -3482,7 +3512,7 @@
       <c r="Z43" s="15"/>
       <c r="AA43" s="17"/>
     </row>
-    <row r="44" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A44" s="21" t="s">
         <v>38</v>
       </c>
@@ -3490,7 +3520,7 @@
         <v>1</v>
       </c>
       <c r="C44" s="34" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D44" s="15"/>
       <c r="E44" s="15" t="s">
@@ -3498,8 +3528,8 @@
       </c>
       <c r="F44" s="15"/>
       <c r="G44" s="16"/>
-      <c r="H44" s="124"/>
-      <c r="I44" s="125"/>
+      <c r="H44" s="100"/>
+      <c r="I44" s="101"/>
       <c r="J44" s="15"/>
       <c r="K44" s="15"/>
       <c r="L44" s="15"/>
@@ -3525,7 +3555,7 @@
       <c r="Z44" s="15"/>
       <c r="AA44" s="17"/>
     </row>
-    <row r="45" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A45" s="21" t="s">
         <v>38</v>
       </c>
@@ -3533,7 +3563,7 @@
         <v>2</v>
       </c>
       <c r="C45" s="34" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D45" s="15" t="s">
         <v>15</v>
@@ -3541,8 +3571,8 @@
       <c r="E45" s="15"/>
       <c r="F45" s="15"/>
       <c r="G45" s="16"/>
-      <c r="H45" s="124"/>
-      <c r="I45" s="125"/>
+      <c r="H45" s="100"/>
+      <c r="I45" s="101"/>
       <c r="J45" s="15"/>
       <c r="K45" s="15"/>
       <c r="L45" s="15"/>
@@ -3568,7 +3598,7 @@
       <c r="Z45" s="15"/>
       <c r="AA45" s="17"/>
     </row>
-    <row r="46" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A46" s="21" t="s">
         <v>38</v>
       </c>
@@ -3576,7 +3606,7 @@
         <v>3</v>
       </c>
       <c r="C46" s="34" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D46" s="15" t="s">
         <v>15</v>
@@ -3586,8 +3616,8 @@
       </c>
       <c r="F46" s="15"/>
       <c r="G46" s="16"/>
-      <c r="H46" s="124"/>
-      <c r="I46" s="125"/>
+      <c r="H46" s="100"/>
+      <c r="I46" s="101"/>
       <c r="J46" s="15"/>
       <c r="K46" s="15"/>
       <c r="L46" s="15"/>
@@ -3607,7 +3637,7 @@
       <c r="Z46" s="15"/>
       <c r="AA46" s="17"/>
     </row>
-    <row r="47" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A47" s="10" t="s">
         <v>40</v>
       </c>
@@ -3615,7 +3645,7 @@
         <v>1</v>
       </c>
       <c r="C47" s="34" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D47" s="15" t="s">
         <v>15</v>
@@ -3623,8 +3653,8 @@
       <c r="E47" s="15"/>
       <c r="F47" s="15"/>
       <c r="G47" s="16"/>
-      <c r="H47" s="124"/>
-      <c r="I47" s="125"/>
+      <c r="H47" s="100"/>
+      <c r="I47" s="101"/>
       <c r="J47" s="15"/>
       <c r="K47" s="15"/>
       <c r="L47" s="15"/>
@@ -3652,9 +3682,9 @@
       <c r="Z47" s="15"/>
       <c r="AA47" s="17"/>
     </row>
-    <row r="48" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A48" s="24" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B48" s="48">
         <v>1</v>
@@ -3674,8 +3704,8 @@
       <c r="G48" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="H48" s="124"/>
-      <c r="I48" s="125"/>
+      <c r="H48" s="100"/>
+      <c r="I48" s="101"/>
       <c r="J48" s="70"/>
       <c r="K48" s="70"/>
       <c r="L48" s="70"/>
@@ -3695,9 +3725,9 @@
       <c r="Z48" s="70"/>
       <c r="AA48" s="17"/>
     </row>
-    <row r="49" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A49" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B49" s="25">
         <v>1</v>
@@ -3717,8 +3747,8 @@
       <c r="G49" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="H49" s="126"/>
-      <c r="I49" s="127"/>
+      <c r="H49" s="102"/>
+      <c r="I49" s="103"/>
       <c r="J49" s="23"/>
       <c r="K49" s="23"/>
       <c r="L49" s="23"/>
@@ -3738,9 +3768,9 @@
       <c r="Z49" s="23"/>
       <c r="AA49" s="25"/>
     </row>
-    <row r="50" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A50" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B50" s="49">
         <v>1</v>
@@ -3760,8 +3790,8 @@
       <c r="G50" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="H50" s="124"/>
-      <c r="I50" s="125"/>
+      <c r="H50" s="100"/>
+      <c r="I50" s="101"/>
       <c r="J50" s="15"/>
       <c r="K50" s="15"/>
       <c r="L50" s="15"/>
@@ -3781,9 +3811,9 @@
       <c r="Z50" s="88"/>
       <c r="AA50" s="89"/>
     </row>
-    <row r="51" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A51" s="13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B51" s="50">
         <v>1</v>
@@ -3797,8 +3827,8 @@
       <c r="E51" s="15"/>
       <c r="F51" s="15"/>
       <c r="G51" s="16"/>
-      <c r="H51" s="124"/>
-      <c r="I51" s="125"/>
+      <c r="H51" s="100"/>
+      <c r="I51" s="101"/>
       <c r="J51" s="15"/>
       <c r="K51" s="15"/>
       <c r="L51" s="15"/>
@@ -3820,15 +3850,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A52" s="26" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B52" s="51">
         <v>1</v>
       </c>
       <c r="C52" s="34" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
@@ -3836,14 +3866,14 @@
         <v>15</v>
       </c>
       <c r="G52" s="22"/>
-      <c r="H52" s="128"/>
-      <c r="I52" s="129"/>
+      <c r="H52" s="104"/>
+      <c r="I52" s="105"/>
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
-      <c r="L52" s="119" t="s">
+      <c r="L52" s="95" t="s">
         <v>11</v>
       </c>
-      <c r="M52" s="119" t="s">
+      <c r="M52" s="95" t="s">
         <v>11</v>
       </c>
       <c r="N52" s="1"/>
@@ -3861,15 +3891,15 @@
       <c r="Z52" s="1"/>
       <c r="AA52" s="3"/>
     </row>
-    <row r="53" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A53" s="27" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B53" s="52">
         <v>1</v>
       </c>
       <c r="C53" s="34" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D53" s="1"/>
       <c r="E53" s="15" t="s">
@@ -3877,14 +3907,14 @@
       </c>
       <c r="F53" s="1"/>
       <c r="G53" s="22"/>
-      <c r="H53" s="128"/>
-      <c r="I53" s="129"/>
+      <c r="H53" s="104"/>
+      <c r="I53" s="105"/>
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
-      <c r="L53" s="114" t="s">
+      <c r="L53" s="90" t="s">
         <v>10</v>
       </c>
-      <c r="M53" s="114" t="s">
+      <c r="M53" s="90" t="s">
         <v>10</v>
       </c>
       <c r="N53" s="1"/>
@@ -3902,15 +3932,15 @@
       <c r="Z53" s="1"/>
       <c r="AA53" s="3"/>
     </row>
-    <row r="54" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A54" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B54" s="53">
         <v>1</v>
       </c>
       <c r="C54" s="34" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D54" s="1"/>
       <c r="E54" s="1" t="s">
@@ -3918,14 +3948,14 @@
       </c>
       <c r="F54" s="1"/>
       <c r="G54" s="22"/>
-      <c r="H54" s="128"/>
-      <c r="I54" s="129"/>
+      <c r="H54" s="104"/>
+      <c r="I54" s="105"/>
       <c r="J54" s="1"/>
       <c r="K54" s="1"/>
-      <c r="L54" s="120" t="s">
+      <c r="L54" s="96" t="s">
         <v>10</v>
       </c>
-      <c r="M54" s="120" t="s">
+      <c r="M54" s="96" t="s">
         <v>10</v>
       </c>
       <c r="N54" s="1"/>
@@ -3943,15 +3973,15 @@
       <c r="Z54" s="1"/>
       <c r="AA54" s="3"/>
     </row>
-    <row r="55" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A55" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B55" s="53">
         <v>2</v>
       </c>
       <c r="C55" s="34" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D55" s="1"/>
       <c r="E55" s="1" t="s">
@@ -3959,15 +3989,15 @@
       </c>
       <c r="F55" s="1"/>
       <c r="G55" s="22"/>
-      <c r="H55" s="128"/>
-      <c r="I55" s="129"/>
+      <c r="H55" s="104"/>
+      <c r="I55" s="105"/>
       <c r="J55" s="1"/>
       <c r="K55" s="1"/>
       <c r="L55" s="1"/>
-      <c r="M55" s="120" t="s">
+      <c r="M55" s="96" t="s">
         <v>10</v>
       </c>
-      <c r="N55" s="120" t="s">
+      <c r="N55" s="96" t="s">
         <v>10</v>
       </c>
       <c r="O55" s="1"/>
@@ -3984,15 +4014,15 @@
       <c r="Z55" s="1"/>
       <c r="AA55" s="3"/>
     </row>
-    <row r="56" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A56" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B56" s="53">
         <v>3</v>
       </c>
       <c r="C56" s="34" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D56" s="1"/>
       <c r="E56" s="1" t="s">
@@ -4000,26 +4030,26 @@
       </c>
       <c r="F56" s="1"/>
       <c r="G56" s="22"/>
-      <c r="H56" s="128"/>
-      <c r="I56" s="129"/>
+      <c r="H56" s="104"/>
+      <c r="I56" s="105"/>
       <c r="J56" s="1"/>
       <c r="K56" s="1"/>
       <c r="L56" s="1"/>
       <c r="M56" s="1"/>
-      <c r="N56" s="120" t="s">
+      <c r="N56" s="96" t="s">
         <v>10</v>
       </c>
-      <c r="O56" s="120" t="s">
+      <c r="O56" s="96" t="s">
         <v>10</v>
       </c>
       <c r="P56" s="1"/>
       <c r="Q56" s="1"/>
       <c r="R56" s="1"/>
       <c r="S56" s="1"/>
-      <c r="T56" s="120" t="s">
+      <c r="T56" s="96" t="s">
         <v>10</v>
       </c>
-      <c r="U56" s="120" t="s">
+      <c r="U56" s="96" t="s">
         <v>10</v>
       </c>
       <c r="V56" s="1"/>
@@ -4029,15 +4059,15 @@
       <c r="Z56" s="1"/>
       <c r="AA56" s="3"/>
     </row>
-    <row r="57" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A57" s="29" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B57" s="54">
         <v>1</v>
       </c>
       <c r="C57" s="34" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D57" s="1"/>
       <c r="E57" s="1" t="s">
@@ -4045,8 +4075,8 @@
       </c>
       <c r="F57" s="1"/>
       <c r="G57" s="22"/>
-      <c r="H57" s="128"/>
-      <c r="I57" s="129"/>
+      <c r="H57" s="104"/>
+      <c r="I57" s="105"/>
       <c r="J57" s="1"/>
       <c r="K57" s="1"/>
       <c r="L57" s="1"/>
@@ -4057,13 +4087,13 @@
       <c r="Q57" s="1"/>
       <c r="R57" s="1"/>
       <c r="S57" s="1"/>
-      <c r="T57" s="121" t="s">
+      <c r="T57" s="97" t="s">
         <v>10</v>
       </c>
-      <c r="U57" s="121" t="s">
+      <c r="U57" s="97" t="s">
         <v>10</v>
       </c>
-      <c r="V57" s="121" t="s">
+      <c r="V57" s="97" t="s">
         <v>10</v>
       </c>
       <c r="W57" s="1"/>
@@ -4072,15 +4102,15 @@
       <c r="Z57" s="1"/>
       <c r="AA57" s="3"/>
     </row>
-    <row r="58" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A58" s="27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B58" s="52">
         <v>1</v>
       </c>
       <c r="C58" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>15</v>
@@ -4088,11 +4118,11 @@
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
       <c r="G58" s="22"/>
-      <c r="H58" s="128"/>
-      <c r="I58" s="129"/>
+      <c r="H58" s="104"/>
+      <c r="I58" s="105"/>
       <c r="J58" s="1"/>
       <c r="K58" s="1"/>
-      <c r="L58" s="114" t="s">
+      <c r="L58" s="90" t="s">
         <v>9</v>
       </c>
       <c r="M58" s="1"/>
@@ -4111,15 +4141,15 @@
       <c r="Z58" s="1"/>
       <c r="AA58" s="3"/>
     </row>
-    <row r="59" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A59" s="27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B59" s="52">
         <v>2</v>
       </c>
       <c r="C59" s="34" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>15</v>
@@ -4131,8 +4161,8 @@
       <c r="G59" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="H59" s="128"/>
-      <c r="I59" s="129"/>
+      <c r="H59" s="104"/>
+      <c r="I59" s="105"/>
       <c r="J59" s="1"/>
       <c r="K59" s="1"/>
       <c r="L59" s="1"/>
@@ -4143,14 +4173,14 @@
       <c r="Q59" s="1"/>
       <c r="R59" s="1"/>
       <c r="S59" s="1"/>
-      <c r="T59" s="114" t="s">
+      <c r="T59" s="90" t="s">
         <v>9</v>
       </c>
-      <c r="U59" s="114" t="s">
-        <v>106</v>
+      <c r="U59" s="90" t="s">
+        <v>105</v>
       </c>
       <c r="V59" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="W59" s="1"/>
       <c r="X59" s="1"/>
@@ -4158,15 +4188,15 @@
       <c r="Z59" s="1"/>
       <c r="AA59" s="3"/>
     </row>
-    <row r="60" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A60" s="27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B60" s="52">
         <v>3</v>
       </c>
       <c r="C60" s="34" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>15</v>
@@ -4178,8 +4208,8 @@
       <c r="G60" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="H60" s="128"/>
-      <c r="I60" s="129"/>
+      <c r="H60" s="104"/>
+      <c r="I60" s="105"/>
       <c r="J60" s="1"/>
       <c r="K60" s="1"/>
       <c r="L60" s="1"/>
@@ -4190,28 +4220,28 @@
       <c r="Q60" s="1"/>
       <c r="R60" s="1"/>
       <c r="S60" s="1"/>
-      <c r="T60" s="114" t="s">
+      <c r="T60" s="90" t="s">
         <v>9</v>
       </c>
-      <c r="U60" s="114" t="s">
-        <v>106</v>
-      </c>
-      <c r="V60" s="114"/>
+      <c r="U60" s="90" t="s">
+        <v>105</v>
+      </c>
+      <c r="V60" s="90"/>
       <c r="W60" s="1"/>
       <c r="X60" s="1"/>
       <c r="Y60" s="1"/>
       <c r="Z60" s="1"/>
       <c r="AA60" s="3"/>
     </row>
-    <row r="61" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A61" s="30" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B61" s="55">
         <v>1</v>
       </c>
       <c r="C61" s="34" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>15</v>
@@ -4221,8 +4251,8 @@
       </c>
       <c r="F61" s="1"/>
       <c r="G61" s="22"/>
-      <c r="H61" s="128"/>
-      <c r="I61" s="129"/>
+      <c r="H61" s="104"/>
+      <c r="I61" s="105"/>
       <c r="J61" s="1"/>
       <c r="K61" s="1"/>
       <c r="L61" s="1"/>
@@ -4236,21 +4266,21 @@
       <c r="T61" s="1"/>
       <c r="U61" s="1"/>
       <c r="V61" s="1"/>
-      <c r="W61" s="115"/>
-      <c r="X61" s="115"/>
+      <c r="W61" s="91"/>
+      <c r="X61" s="91"/>
       <c r="Y61" s="1"/>
       <c r="Z61" s="1"/>
       <c r="AA61" s="3"/>
     </row>
-    <row r="62" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A62" s="31" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B62" s="56">
         <v>1</v>
       </c>
       <c r="C62" s="34" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>15</v>
@@ -4260,8 +4290,8 @@
       </c>
       <c r="F62" s="1"/>
       <c r="G62" s="22"/>
-      <c r="H62" s="128"/>
-      <c r="I62" s="129"/>
+      <c r="H62" s="104"/>
+      <c r="I62" s="105"/>
       <c r="J62" s="1"/>
       <c r="K62" s="1"/>
       <c r="L62" s="1"/>
@@ -4276,20 +4306,20 @@
       <c r="U62" s="1"/>
       <c r="V62" s="1"/>
       <c r="W62" s="1"/>
-      <c r="X62" s="116"/>
-      <c r="Y62" s="116"/>
+      <c r="X62" s="92"/>
+      <c r="Y62" s="92"/>
       <c r="Z62" s="1"/>
       <c r="AA62" s="3"/>
     </row>
-    <row r="63" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A63" s="32" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B63" s="57">
         <v>1</v>
       </c>
       <c r="C63" s="34" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D63" s="1"/>
       <c r="E63" s="1" t="s">
@@ -4301,36 +4331,36 @@
       <c r="G63" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="H63" s="128"/>
-      <c r="I63" s="129"/>
+      <c r="H63" s="104"/>
+      <c r="I63" s="105"/>
       <c r="J63" s="1"/>
       <c r="K63" s="1"/>
-      <c r="L63" s="117"/>
-      <c r="M63" s="117"/>
-      <c r="N63" s="117"/>
-      <c r="O63" s="117"/>
-      <c r="P63" s="117"/>
-      <c r="Q63" s="117"/>
-      <c r="R63" s="117"/>
-      <c r="S63" s="117"/>
-      <c r="T63" s="117"/>
-      <c r="U63" s="117"/>
-      <c r="V63" s="117"/>
-      <c r="W63" s="117"/>
-      <c r="X63" s="117"/>
-      <c r="Y63" s="117"/>
+      <c r="L63" s="93"/>
+      <c r="M63" s="93"/>
+      <c r="N63" s="93"/>
+      <c r="O63" s="93"/>
+      <c r="P63" s="93"/>
+      <c r="Q63" s="93"/>
+      <c r="R63" s="93"/>
+      <c r="S63" s="93"/>
+      <c r="T63" s="93"/>
+      <c r="U63" s="93"/>
+      <c r="V63" s="93"/>
+      <c r="W63" s="93"/>
+      <c r="X63" s="93"/>
+      <c r="Y63" s="93"/>
       <c r="Z63" s="1"/>
       <c r="AA63" s="3"/>
     </row>
-    <row r="64" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A64" s="33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B64" s="58">
         <v>1</v>
       </c>
       <c r="C64" s="34" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>15</v>
@@ -4344,33 +4374,33 @@
       <c r="G64" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="H64" s="128"/>
-      <c r="I64" s="129"/>
+      <c r="H64" s="104"/>
+      <c r="I64" s="105"/>
       <c r="J64" s="1"/>
       <c r="K64" s="1"/>
       <c r="L64" s="1"/>
-      <c r="M64" s="118"/>
-      <c r="N64" s="118"/>
-      <c r="O64" s="118"/>
-      <c r="P64" s="118"/>
-      <c r="Q64" s="118"/>
-      <c r="R64" s="118"/>
-      <c r="S64" s="118"/>
-      <c r="T64" s="118"/>
-      <c r="U64" s="118"/>
-      <c r="V64" s="118"/>
-      <c r="W64" s="118"/>
-      <c r="X64" s="118"/>
-      <c r="Y64" s="118"/>
+      <c r="M64" s="94"/>
+      <c r="N64" s="94"/>
+      <c r="O64" s="94"/>
+      <c r="P64" s="94"/>
+      <c r="Q64" s="94"/>
+      <c r="R64" s="94"/>
+      <c r="S64" s="94"/>
+      <c r="T64" s="94"/>
+      <c r="U64" s="94"/>
+      <c r="V64" s="94"/>
+      <c r="W64" s="94"/>
+      <c r="X64" s="94"/>
+      <c r="Y64" s="94"/>
       <c r="Z64" s="1"/>
       <c r="AA64" s="3"/>
     </row>
-    <row r="65" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A65" s="90" t="e">
+    <row r="65" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="106" t="e">
         <f>+B38:AA68</f>
         <v>#VALUE!</v>
       </c>
-      <c r="B65" s="91"/>
+      <c r="B65" s="107"/>
       <c r="C65" s="35" t="s">
         <v>42</v>
       </c>
@@ -4390,28 +4420,28 @@
         <f>COUNTIF(G5:G64, "X")</f>
         <v>26</v>
       </c>
-      <c r="H65" s="92"/>
-      <c r="I65" s="92"/>
-      <c r="J65" s="92"/>
-      <c r="K65" s="92"/>
-      <c r="L65" s="92"/>
-      <c r="M65" s="92"/>
-      <c r="N65" s="92"/>
-      <c r="O65" s="92"/>
-      <c r="P65" s="92"/>
-      <c r="Q65" s="92"/>
-      <c r="R65" s="92"/>
-      <c r="S65" s="92"/>
-      <c r="T65" s="92"/>
-      <c r="U65" s="92"/>
-      <c r="V65" s="92"/>
-      <c r="W65" s="92"/>
-      <c r="X65" s="92"/>
-      <c r="Y65" s="92"/>
-      <c r="Z65" s="92"/>
-      <c r="AA65" s="93"/>
-    </row>
-    <row r="66" spans="1:27" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+      <c r="H65" s="108"/>
+      <c r="I65" s="108"/>
+      <c r="J65" s="108"/>
+      <c r="K65" s="108"/>
+      <c r="L65" s="108"/>
+      <c r="M65" s="108"/>
+      <c r="N65" s="108"/>
+      <c r="O65" s="108"/>
+      <c r="P65" s="108"/>
+      <c r="Q65" s="108"/>
+      <c r="R65" s="108"/>
+      <c r="S65" s="108"/>
+      <c r="T65" s="108"/>
+      <c r="U65" s="108"/>
+      <c r="V65" s="108"/>
+      <c r="W65" s="108"/>
+      <c r="X65" s="108"/>
+      <c r="Y65" s="108"/>
+      <c r="Z65" s="108"/>
+      <c r="AA65" s="109"/>
+    </row>
+    <row r="66" spans="1:27" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="11">
     <mergeCell ref="A65:B65"/>

</xml_diff>

<commit_message>
Modified and corrected attack, read desc
-He creado una funcion que ya existia y que era de raquel , asi que ahora la nueva tb es de raquel
-Modificado attack, ahora no necesita alocar memoria y necesita un argumento
</commit_message>
<xml_diff>
--- a/Reuniones_Coordinacion/Diagrama_Gantt_8_4_25_Saul_Fernando_Raquel_Irene.xlsx
+++ b/Reuniones_Coordinacion/Diagrama_Gantt_8_4_25_Saul_Fernando_Raquel_Irene.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\fernandpo\cosa_uni\proyecto_program\Reuniones_Coordinacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C79EA513-F26B-4A97-8823-4751DF0038F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB666928-3DC9-4737-87E4-487A68CFCB77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{76F30C29-DD84-4491-9B4C-00A38B383DA8}"/>
   </bookViews>
@@ -1231,6 +1231,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1301,12 +1307,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1690,8 +1690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13B8C02F-838E-4995-8CF9-185661B72170}">
   <dimension ref="A1:AA66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="135" zoomScaleNormal="135" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="135" zoomScaleNormal="135" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1706,114 +1706,114 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="110" t="s">
+      <c r="A1" s="112" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="111"/>
-      <c r="C1" s="111"/>
-      <c r="D1" s="111"/>
-      <c r="E1" s="111"/>
-      <c r="F1" s="111"/>
-      <c r="G1" s="111"/>
-      <c r="H1" s="111"/>
-      <c r="I1" s="111"/>
-      <c r="J1" s="111"/>
-      <c r="K1" s="111"/>
-      <c r="L1" s="111"/>
-      <c r="M1" s="111"/>
-      <c r="N1" s="111"/>
-      <c r="O1" s="111"/>
-      <c r="P1" s="111"/>
-      <c r="Q1" s="111"/>
-      <c r="R1" s="111"/>
-      <c r="S1" s="111"/>
-      <c r="T1" s="111"/>
-      <c r="U1" s="111"/>
-      <c r="V1" s="111"/>
-      <c r="W1" s="111"/>
-      <c r="X1" s="111"/>
-      <c r="Y1" s="111"/>
-      <c r="Z1" s="111"/>
-      <c r="AA1" s="112"/>
+      <c r="B1" s="113"/>
+      <c r="C1" s="113"/>
+      <c r="D1" s="113"/>
+      <c r="E1" s="113"/>
+      <c r="F1" s="113"/>
+      <c r="G1" s="113"/>
+      <c r="H1" s="113"/>
+      <c r="I1" s="113"/>
+      <c r="J1" s="113"/>
+      <c r="K1" s="113"/>
+      <c r="L1" s="113"/>
+      <c r="M1" s="113"/>
+      <c r="N1" s="113"/>
+      <c r="O1" s="113"/>
+      <c r="P1" s="113"/>
+      <c r="Q1" s="113"/>
+      <c r="R1" s="113"/>
+      <c r="S1" s="113"/>
+      <c r="T1" s="113"/>
+      <c r="U1" s="113"/>
+      <c r="V1" s="113"/>
+      <c r="W1" s="113"/>
+      <c r="X1" s="113"/>
+      <c r="Y1" s="113"/>
+      <c r="Z1" s="113"/>
+      <c r="AA1" s="114"/>
     </row>
     <row r="2" spans="1:27" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="113" t="s">
+      <c r="A2" s="115" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="114"/>
-      <c r="C2" s="119" t="s">
+      <c r="B2" s="116"/>
+      <c r="C2" s="121" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="122" t="s">
+      <c r="D2" s="124" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="122"/>
-      <c r="F2" s="122"/>
-      <c r="G2" s="123"/>
-      <c r="H2" s="126" t="s">
+      <c r="E2" s="124"/>
+      <c r="F2" s="124"/>
+      <c r="G2" s="125"/>
+      <c r="H2" s="128" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="122"/>
-      <c r="J2" s="122"/>
-      <c r="K2" s="122"/>
-      <c r="L2" s="122"/>
-      <c r="M2" s="122"/>
-      <c r="N2" s="122"/>
-      <c r="O2" s="122"/>
-      <c r="P2" s="122"/>
-      <c r="Q2" s="122"/>
-      <c r="R2" s="122"/>
-      <c r="S2" s="122"/>
-      <c r="T2" s="122"/>
-      <c r="U2" s="122"/>
-      <c r="V2" s="122"/>
-      <c r="W2" s="122"/>
-      <c r="X2" s="122"/>
-      <c r="Y2" s="122"/>
-      <c r="Z2" s="122"/>
-      <c r="AA2" s="127"/>
+      <c r="I2" s="124"/>
+      <c r="J2" s="124"/>
+      <c r="K2" s="124"/>
+      <c r="L2" s="124"/>
+      <c r="M2" s="124"/>
+      <c r="N2" s="124"/>
+      <c r="O2" s="124"/>
+      <c r="P2" s="124"/>
+      <c r="Q2" s="124"/>
+      <c r="R2" s="124"/>
+      <c r="S2" s="124"/>
+      <c r="T2" s="124"/>
+      <c r="U2" s="124"/>
+      <c r="V2" s="124"/>
+      <c r="W2" s="124"/>
+      <c r="X2" s="124"/>
+      <c r="Y2" s="124"/>
+      <c r="Z2" s="124"/>
+      <c r="AA2" s="129"/>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A3" s="115"/>
-      <c r="B3" s="116"/>
-      <c r="C3" s="120"/>
-      <c r="D3" s="124"/>
-      <c r="E3" s="124"/>
-      <c r="F3" s="124"/>
-      <c r="G3" s="125"/>
-      <c r="H3" s="128" t="s">
+      <c r="A3" s="117"/>
+      <c r="B3" s="118"/>
+      <c r="C3" s="122"/>
+      <c r="D3" s="126"/>
+      <c r="E3" s="126"/>
+      <c r="F3" s="126"/>
+      <c r="G3" s="127"/>
+      <c r="H3" s="130" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="124"/>
-      <c r="J3" s="124"/>
-      <c r="K3" s="124"/>
-      <c r="L3" s="124"/>
-      <c r="M3" s="124" t="s">
+      <c r="I3" s="126"/>
+      <c r="J3" s="126"/>
+      <c r="K3" s="126"/>
+      <c r="L3" s="126"/>
+      <c r="M3" s="126" t="s">
         <v>6</v>
       </c>
-      <c r="N3" s="124"/>
-      <c r="O3" s="124"/>
-      <c r="P3" s="124"/>
-      <c r="Q3" s="124"/>
-      <c r="R3" s="124" t="s">
+      <c r="N3" s="126"/>
+      <c r="O3" s="126"/>
+      <c r="P3" s="126"/>
+      <c r="Q3" s="126"/>
+      <c r="R3" s="126" t="s">
         <v>7</v>
       </c>
-      <c r="S3" s="124"/>
-      <c r="T3" s="124"/>
-      <c r="U3" s="124"/>
-      <c r="V3" s="124"/>
-      <c r="W3" s="124" t="s">
+      <c r="S3" s="126"/>
+      <c r="T3" s="126"/>
+      <c r="U3" s="126"/>
+      <c r="V3" s="126"/>
+      <c r="W3" s="126" t="s">
         <v>8</v>
       </c>
-      <c r="X3" s="124"/>
-      <c r="Y3" s="124"/>
-      <c r="Z3" s="124"/>
-      <c r="AA3" s="129"/>
+      <c r="X3" s="126"/>
+      <c r="Y3" s="126"/>
+      <c r="Z3" s="126"/>
+      <c r="AA3" s="131"/>
     </row>
     <row r="4" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="117"/>
-      <c r="B4" s="118"/>
-      <c r="C4" s="121"/>
+      <c r="A4" s="119"/>
+      <c r="B4" s="120"/>
+      <c r="C4" s="123"/>
       <c r="D4" s="66" t="s">
         <v>9</v>
       </c>
@@ -2164,7 +2164,7 @@
       <c r="D11" s="15"/>
       <c r="E11" s="15"/>
       <c r="F11" s="15"/>
-      <c r="G11" s="16" t="s">
+      <c r="G11" s="106" t="s">
         <v>15</v>
       </c>
       <c r="H11" s="100"/>
@@ -2241,7 +2241,7 @@
       </c>
       <c r="D13" s="15"/>
       <c r="E13" s="15"/>
-      <c r="F13" s="15" t="s">
+      <c r="F13" s="106" t="s">
         <v>15</v>
       </c>
       <c r="G13" s="16"/>
@@ -2280,7 +2280,7 @@
       </c>
       <c r="D14" s="15"/>
       <c r="E14" s="15"/>
-      <c r="F14" s="15" t="s">
+      <c r="F14" s="106" t="s">
         <v>15</v>
       </c>
       <c r="G14" s="16"/>
@@ -2437,7 +2437,7 @@
       <c r="D18" s="15"/>
       <c r="E18" s="15"/>
       <c r="F18" s="15"/>
-      <c r="G18" s="130" t="s">
+      <c r="G18" s="106" t="s">
         <v>15</v>
       </c>
       <c r="H18" s="100"/>
@@ -2476,7 +2476,7 @@
       <c r="D19" s="15"/>
       <c r="E19" s="15"/>
       <c r="F19" s="15"/>
-      <c r="G19" s="16" t="s">
+      <c r="G19" s="106" t="s">
         <v>15</v>
       </c>
       <c r="H19" s="100"/>
@@ -2517,7 +2517,7 @@
       <c r="D20" s="15"/>
       <c r="E20" s="15"/>
       <c r="F20" s="15"/>
-      <c r="G20" s="131" t="s">
+      <c r="G20" s="107" t="s">
         <v>15</v>
       </c>
       <c r="H20" s="100"/>
@@ -2558,7 +2558,7 @@
       <c r="D21" s="15"/>
       <c r="E21" s="15"/>
       <c r="F21" s="15"/>
-      <c r="G21" s="16" t="s">
+      <c r="G21" s="106" t="s">
         <v>15</v>
       </c>
       <c r="H21" s="100"/>
@@ -4396,11 +4396,11 @@
       <c r="AA64" s="3"/>
     </row>
     <row r="65" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="106" t="e">
+      <c r="A65" s="108" t="e">
         <f>+B38:AA68</f>
         <v>#VALUE!</v>
       </c>
-      <c r="B65" s="107"/>
+      <c r="B65" s="109"/>
       <c r="C65" s="35" t="s">
         <v>42</v>
       </c>
@@ -4420,26 +4420,26 @@
         <f>COUNTIF(G5:G64, "X")</f>
         <v>26</v>
       </c>
-      <c r="H65" s="108"/>
-      <c r="I65" s="108"/>
-      <c r="J65" s="108"/>
-      <c r="K65" s="108"/>
-      <c r="L65" s="108"/>
-      <c r="M65" s="108"/>
-      <c r="N65" s="108"/>
-      <c r="O65" s="108"/>
-      <c r="P65" s="108"/>
-      <c r="Q65" s="108"/>
-      <c r="R65" s="108"/>
-      <c r="S65" s="108"/>
-      <c r="T65" s="108"/>
-      <c r="U65" s="108"/>
-      <c r="V65" s="108"/>
-      <c r="W65" s="108"/>
-      <c r="X65" s="108"/>
-      <c r="Y65" s="108"/>
-      <c r="Z65" s="108"/>
-      <c r="AA65" s="109"/>
+      <c r="H65" s="110"/>
+      <c r="I65" s="110"/>
+      <c r="J65" s="110"/>
+      <c r="K65" s="110"/>
+      <c r="L65" s="110"/>
+      <c r="M65" s="110"/>
+      <c r="N65" s="110"/>
+      <c r="O65" s="110"/>
+      <c r="P65" s="110"/>
+      <c r="Q65" s="110"/>
+      <c r="R65" s="110"/>
+      <c r="S65" s="110"/>
+      <c r="T65" s="110"/>
+      <c r="U65" s="110"/>
+      <c r="V65" s="110"/>
+      <c r="W65" s="110"/>
+      <c r="X65" s="110"/>
+      <c r="Y65" s="110"/>
+      <c r="Z65" s="110"/>
+      <c r="AA65" s="111"/>
     </row>
     <row r="66" spans="1:27" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>

</xml_diff>

<commit_message>
Aprendido el arte de BASH + hecho la cosa que se entrega el martes 👍
</commit_message>
<xml_diff>
--- a/Reuniones_Coordinacion/Diagrama_Gantt_8_4_25_Saul_Fernando_Raquel_Irene.xlsx
+++ b/Reuniones_Coordinacion/Diagrama_Gantt_8_4_25_Saul_Fernando_Raquel_Irene.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\fernandpo\cosa_uni\proyecto_program\Reuniones_Coordinacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\saul\Pprog_conversation\Reuniones_Coordinacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CDC97FB-2A72-40E7-A1B5-2427DF070493}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B0C54B4-6490-4493-BDD1-A802A3F51C28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{76F30C29-DD84-4491-9B4C-00A38B383DA8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{76F30C29-DD84-4491-9B4C-00A38B383DA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,17 +19,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1237,6 +1226,9 @@
     <xf numFmtId="0" fontId="1" fillId="26" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1307,9 +1299,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1395,9 +1384,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1435,7 +1424,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1541,7 +1530,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1683,7 +1672,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1693,130 +1682,130 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13B8C02F-838E-4995-8CF9-185661B72170}">
   <dimension ref="A1:AA66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="120" zoomScaleNormal="135" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="135" workbookViewId="0">
+      <selection activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.08984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="3.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="3.08984375" bestFit="1" customWidth="1"/>
     <col min="8" max="24" width="3" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="2.88671875" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="2.90625" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="112" t="s">
+    <row r="1" spans="1:27" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="113" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="113"/>
-      <c r="C1" s="113"/>
-      <c r="D1" s="113"/>
-      <c r="E1" s="113"/>
-      <c r="F1" s="113"/>
-      <c r="G1" s="113"/>
-      <c r="H1" s="113"/>
-      <c r="I1" s="113"/>
-      <c r="J1" s="113"/>
-      <c r="K1" s="113"/>
-      <c r="L1" s="113"/>
-      <c r="M1" s="113"/>
-      <c r="N1" s="113"/>
-      <c r="O1" s="113"/>
-      <c r="P1" s="113"/>
-      <c r="Q1" s="113"/>
-      <c r="R1" s="113"/>
-      <c r="S1" s="113"/>
-      <c r="T1" s="113"/>
-      <c r="U1" s="113"/>
-      <c r="V1" s="113"/>
-      <c r="W1" s="113"/>
-      <c r="X1" s="113"/>
-      <c r="Y1" s="113"/>
-      <c r="Z1" s="113"/>
-      <c r="AA1" s="114"/>
-    </row>
-    <row r="2" spans="1:27" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="115" t="s">
+      <c r="B1" s="114"/>
+      <c r="C1" s="114"/>
+      <c r="D1" s="114"/>
+      <c r="E1" s="114"/>
+      <c r="F1" s="114"/>
+      <c r="G1" s="114"/>
+      <c r="H1" s="114"/>
+      <c r="I1" s="114"/>
+      <c r="J1" s="114"/>
+      <c r="K1" s="114"/>
+      <c r="L1" s="114"/>
+      <c r="M1" s="114"/>
+      <c r="N1" s="114"/>
+      <c r="O1" s="114"/>
+      <c r="P1" s="114"/>
+      <c r="Q1" s="114"/>
+      <c r="R1" s="114"/>
+      <c r="S1" s="114"/>
+      <c r="T1" s="114"/>
+      <c r="U1" s="114"/>
+      <c r="V1" s="114"/>
+      <c r="W1" s="114"/>
+      <c r="X1" s="114"/>
+      <c r="Y1" s="114"/>
+      <c r="Z1" s="114"/>
+      <c r="AA1" s="115"/>
+    </row>
+    <row r="2" spans="1:27" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="116" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="116"/>
-      <c r="C2" s="121" t="s">
+      <c r="B2" s="117"/>
+      <c r="C2" s="122" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="124" t="s">
+      <c r="D2" s="125" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="124"/>
-      <c r="F2" s="124"/>
-      <c r="G2" s="125"/>
-      <c r="H2" s="128" t="s">
+      <c r="E2" s="125"/>
+      <c r="F2" s="125"/>
+      <c r="G2" s="126"/>
+      <c r="H2" s="129" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="124"/>
-      <c r="J2" s="124"/>
-      <c r="K2" s="124"/>
-      <c r="L2" s="124"/>
-      <c r="M2" s="124"/>
-      <c r="N2" s="124"/>
-      <c r="O2" s="124"/>
-      <c r="P2" s="124"/>
-      <c r="Q2" s="124"/>
-      <c r="R2" s="124"/>
-      <c r="S2" s="124"/>
-      <c r="T2" s="124"/>
-      <c r="U2" s="124"/>
-      <c r="V2" s="124"/>
-      <c r="W2" s="124"/>
-      <c r="X2" s="124"/>
-      <c r="Y2" s="124"/>
-      <c r="Z2" s="124"/>
-      <c r="AA2" s="129"/>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A3" s="117"/>
-      <c r="B3" s="118"/>
-      <c r="C3" s="122"/>
-      <c r="D3" s="126"/>
-      <c r="E3" s="126"/>
-      <c r="F3" s="126"/>
-      <c r="G3" s="127"/>
-      <c r="H3" s="130" t="s">
+      <c r="I2" s="125"/>
+      <c r="J2" s="125"/>
+      <c r="K2" s="125"/>
+      <c r="L2" s="125"/>
+      <c r="M2" s="125"/>
+      <c r="N2" s="125"/>
+      <c r="O2" s="125"/>
+      <c r="P2" s="125"/>
+      <c r="Q2" s="125"/>
+      <c r="R2" s="125"/>
+      <c r="S2" s="125"/>
+      <c r="T2" s="125"/>
+      <c r="U2" s="125"/>
+      <c r="V2" s="125"/>
+      <c r="W2" s="125"/>
+      <c r="X2" s="125"/>
+      <c r="Y2" s="125"/>
+      <c r="Z2" s="125"/>
+      <c r="AA2" s="130"/>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A3" s="118"/>
+      <c r="B3" s="119"/>
+      <c r="C3" s="123"/>
+      <c r="D3" s="127"/>
+      <c r="E3" s="127"/>
+      <c r="F3" s="127"/>
+      <c r="G3" s="128"/>
+      <c r="H3" s="131" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="126"/>
-      <c r="J3" s="126"/>
-      <c r="K3" s="126"/>
-      <c r="L3" s="126"/>
-      <c r="M3" s="126" t="s">
+      <c r="I3" s="127"/>
+      <c r="J3" s="127"/>
+      <c r="K3" s="127"/>
+      <c r="L3" s="127"/>
+      <c r="M3" s="127" t="s">
         <v>6</v>
       </c>
-      <c r="N3" s="126"/>
-      <c r="O3" s="126"/>
-      <c r="P3" s="126"/>
-      <c r="Q3" s="126"/>
-      <c r="R3" s="126" t="s">
+      <c r="N3" s="127"/>
+      <c r="O3" s="127"/>
+      <c r="P3" s="127"/>
+      <c r="Q3" s="127"/>
+      <c r="R3" s="127" t="s">
         <v>7</v>
       </c>
-      <c r="S3" s="126"/>
-      <c r="T3" s="126"/>
-      <c r="U3" s="126"/>
-      <c r="V3" s="126"/>
-      <c r="W3" s="126" t="s">
+      <c r="S3" s="127"/>
+      <c r="T3" s="127"/>
+      <c r="U3" s="127"/>
+      <c r="V3" s="127"/>
+      <c r="W3" s="127" t="s">
         <v>8</v>
       </c>
-      <c r="X3" s="126"/>
-      <c r="Y3" s="126"/>
-      <c r="Z3" s="126"/>
-      <c r="AA3" s="131"/>
-    </row>
-    <row r="4" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="119"/>
-      <c r="B4" s="120"/>
-      <c r="C4" s="123"/>
+      <c r="X3" s="127"/>
+      <c r="Y3" s="127"/>
+      <c r="Z3" s="127"/>
+      <c r="AA3" s="132"/>
+    </row>
+    <row r="4" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="120"/>
+      <c r="B4" s="121"/>
+      <c r="C4" s="124"/>
       <c r="D4" s="66" t="s">
         <v>9</v>
       </c>
@@ -1890,7 +1879,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A5" s="59" t="s">
         <v>13</v>
       </c>
@@ -1933,7 +1922,7 @@
       <c r="Z5" s="64"/>
       <c r="AA5" s="65"/>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
@@ -1972,7 +1961,7 @@
       <c r="Z6" s="71"/>
       <c r="AA6" s="17"/>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
@@ -2015,7 +2004,7 @@
       <c r="Z7" s="71"/>
       <c r="AA7" s="17"/>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
@@ -2058,7 +2047,7 @@
       <c r="Z8" s="71"/>
       <c r="AA8" s="17"/>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>20</v>
       </c>
@@ -2109,7 +2098,7 @@
       <c r="Z9" s="72"/>
       <c r="AA9" s="17"/>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>20</v>
       </c>
@@ -2154,7 +2143,7 @@
       <c r="Z10" s="72"/>
       <c r="AA10" s="17"/>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>23</v>
       </c>
@@ -2193,7 +2182,7 @@
       <c r="Z11" s="15"/>
       <c r="AA11" s="17"/>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>23</v>
       </c>
@@ -2232,7 +2221,7 @@
       <c r="Z12" s="15"/>
       <c r="AA12" s="17"/>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A13" s="18" t="s">
         <v>24</v>
       </c>
@@ -2271,7 +2260,7 @@
       <c r="Z13" s="15"/>
       <c r="AA13" s="17"/>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A14" s="18" t="s">
         <v>24</v>
       </c>
@@ -2310,7 +2299,7 @@
       <c r="Z14" s="15"/>
       <c r="AA14" s="17"/>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A15" s="18" t="s">
         <v>24</v>
       </c>
@@ -2349,7 +2338,7 @@
       <c r="Z15" s="15"/>
       <c r="AA15" s="17"/>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A16" s="19" t="s">
         <v>25</v>
       </c>
@@ -2388,7 +2377,7 @@
       <c r="Z16" s="15"/>
       <c r="AA16" s="17"/>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A17" s="19" t="s">
         <v>25</v>
       </c>
@@ -2427,7 +2416,7 @@
       <c r="Z17" s="15"/>
       <c r="AA17" s="17"/>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A18" s="77" t="s">
         <v>26</v>
       </c>
@@ -2466,7 +2455,7 @@
       <c r="Z18" s="15"/>
       <c r="AA18" s="17"/>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A19" s="77" t="s">
         <v>26</v>
       </c>
@@ -2507,7 +2496,7 @@
       <c r="Z19" s="15"/>
       <c r="AA19" s="17"/>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A20" s="77" t="s">
         <v>26</v>
       </c>
@@ -2548,7 +2537,7 @@
       <c r="Z20" s="15"/>
       <c r="AA20" s="17"/>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A21" s="77" t="s">
         <v>26</v>
       </c>
@@ -2591,7 +2580,7 @@
       <c r="Z21" s="15"/>
       <c r="AA21" s="17"/>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>27</v>
       </c>
@@ -2630,7 +2619,7 @@
       <c r="Z22" s="15"/>
       <c r="AA22" s="17"/>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>27</v>
       </c>
@@ -2669,7 +2658,7 @@
       <c r="Z23" s="15"/>
       <c r="AA23" s="17"/>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>27</v>
       </c>
@@ -2714,7 +2703,7 @@
       <c r="Z24" s="15"/>
       <c r="AA24" s="17"/>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A25" s="6" t="s">
         <v>28</v>
       </c>
@@ -2725,7 +2714,7 @@
         <v>56</v>
       </c>
       <c r="D25" s="15"/>
-      <c r="E25" s="132" t="s">
+      <c r="E25" s="108" t="s">
         <v>15</v>
       </c>
       <c r="F25" s="15"/>
@@ -2753,7 +2742,7 @@
       <c r="Z25" s="15"/>
       <c r="AA25" s="17"/>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A26" s="6" t="s">
         <v>28</v>
       </c>
@@ -2764,7 +2753,7 @@
         <v>57</v>
       </c>
       <c r="D26" s="15"/>
-      <c r="E26" s="132" t="s">
+      <c r="E26" s="108" t="s">
         <v>15</v>
       </c>
       <c r="F26" s="15"/>
@@ -2792,7 +2781,7 @@
       <c r="Z26" s="15"/>
       <c r="AA26" s="17"/>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A27" s="6" t="s">
         <v>28</v>
       </c>
@@ -2803,7 +2792,7 @@
         <v>58</v>
       </c>
       <c r="D27" s="15"/>
-      <c r="E27" s="132" t="s">
+      <c r="E27" s="108" t="s">
         <v>15</v>
       </c>
       <c r="F27" s="15"/>
@@ -2831,7 +2820,7 @@
       <c r="Z27" s="15"/>
       <c r="AA27" s="17"/>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A28" s="80" t="s">
         <v>29</v>
       </c>
@@ -2874,7 +2863,7 @@
       <c r="Z28" s="15"/>
       <c r="AA28" s="17"/>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A29" s="7" t="s">
         <v>30</v>
       </c>
@@ -2915,7 +2904,7 @@
       <c r="Z29" s="15"/>
       <c r="AA29" s="17"/>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A30" s="7" t="s">
         <v>30</v>
       </c>
@@ -2956,7 +2945,7 @@
       <c r="Z30" s="15"/>
       <c r="AA30" s="17"/>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A31" s="8" t="s">
         <v>31</v>
       </c>
@@ -2995,7 +2984,7 @@
       <c r="Z31" s="15"/>
       <c r="AA31" s="17"/>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A32" s="18" t="s">
         <v>32</v>
       </c>
@@ -3038,7 +3027,7 @@
       <c r="Z32" s="15"/>
       <c r="AA32" s="17"/>
     </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A33" s="18" t="s">
         <v>32</v>
       </c>
@@ -3085,7 +3074,7 @@
       <c r="Z33" s="15"/>
       <c r="AA33" s="17"/>
     </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A34" s="10" t="s">
         <v>33</v>
       </c>
@@ -3122,7 +3111,7 @@
       <c r="Z34" s="15"/>
       <c r="AA34" s="17"/>
     </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A35" s="10" t="s">
         <v>33</v>
       </c>
@@ -3163,7 +3152,7 @@
       <c r="Z35" s="15"/>
       <c r="AA35" s="17"/>
     </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A36" s="10" t="s">
         <v>33</v>
       </c>
@@ -3204,7 +3193,7 @@
       <c r="Z36" s="15"/>
       <c r="AA36" s="17"/>
     </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A37" s="10" t="s">
         <v>33</v>
       </c>
@@ -3249,7 +3238,7 @@
       <c r="Z37" s="15"/>
       <c r="AA37" s="17"/>
     </row>
-    <row r="38" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A38" s="10" t="s">
         <v>33</v>
       </c>
@@ -3259,7 +3248,7 @@
       <c r="C38" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="D38" s="15" t="s">
+      <c r="D38" s="106" t="s">
         <v>15</v>
       </c>
       <c r="E38" s="15" t="s">
@@ -3296,7 +3285,7 @@
       <c r="Z38" s="15"/>
       <c r="AA38" s="17"/>
     </row>
-    <row r="39" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A39" s="9" t="s">
         <v>34</v>
       </c>
@@ -3306,7 +3295,7 @@
       <c r="C39" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="D39" s="15" t="s">
+      <c r="D39" s="106" t="s">
         <v>15</v>
       </c>
       <c r="E39" s="15"/>
@@ -3337,7 +3326,7 @@
       <c r="Z39" s="15"/>
       <c r="AA39" s="17"/>
     </row>
-    <row r="40" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A40" s="9" t="s">
         <v>34</v>
       </c>
@@ -3347,7 +3336,7 @@
       <c r="C40" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="D40" s="15" t="s">
+      <c r="D40" s="106" t="s">
         <v>15</v>
       </c>
       <c r="E40" s="15"/>
@@ -3382,7 +3371,7 @@
       <c r="Z40" s="15"/>
       <c r="AA40" s="17"/>
     </row>
-    <row r="41" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A41" s="9" t="s">
         <v>34</v>
       </c>
@@ -3392,7 +3381,7 @@
       <c r="C41" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="D41" s="15" t="s">
+      <c r="D41" s="106" t="s">
         <v>15</v>
       </c>
       <c r="E41" s="15"/>
@@ -3427,7 +3416,7 @@
       <c r="Z41" s="15"/>
       <c r="AA41" s="17"/>
     </row>
-    <row r="42" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A42" s="9" t="s">
         <v>34</v>
       </c>
@@ -3437,7 +3426,7 @@
       <c r="C42" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="D42" s="15" t="s">
+      <c r="D42" s="106" t="s">
         <v>15</v>
       </c>
       <c r="E42" s="15"/>
@@ -3476,7 +3465,7 @@
       <c r="Z42" s="15"/>
       <c r="AA42" s="17"/>
     </row>
-    <row r="43" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A43" s="20" t="s">
         <v>36</v>
       </c>
@@ -3515,7 +3504,7 @@
       <c r="Z43" s="15"/>
       <c r="AA43" s="17"/>
     </row>
-    <row r="44" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A44" s="21" t="s">
         <v>38</v>
       </c>
@@ -3558,7 +3547,7 @@
       <c r="Z44" s="15"/>
       <c r="AA44" s="17"/>
     </row>
-    <row r="45" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A45" s="21" t="s">
         <v>38</v>
       </c>
@@ -3601,7 +3590,7 @@
       <c r="Z45" s="15"/>
       <c r="AA45" s="17"/>
     </row>
-    <row r="46" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A46" s="21" t="s">
         <v>38</v>
       </c>
@@ -3640,7 +3629,7 @@
       <c r="Z46" s="15"/>
       <c r="AA46" s="17"/>
     </row>
-    <row r="47" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A47" s="10" t="s">
         <v>40</v>
       </c>
@@ -3685,7 +3674,7 @@
       <c r="Z47" s="15"/>
       <c r="AA47" s="17"/>
     </row>
-    <row r="48" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A48" s="24" t="s">
         <v>78</v>
       </c>
@@ -3728,7 +3717,7 @@
       <c r="Z48" s="70"/>
       <c r="AA48" s="17"/>
     </row>
-    <row r="49" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A49" s="11" t="s">
         <v>79</v>
       </c>
@@ -3771,7 +3760,7 @@
       <c r="Z49" s="23"/>
       <c r="AA49" s="25"/>
     </row>
-    <row r="50" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A50" s="12" t="s">
         <v>80</v>
       </c>
@@ -3814,7 +3803,7 @@
       <c r="Z50" s="88"/>
       <c r="AA50" s="89"/>
     </row>
-    <row r="51" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A51" s="13" t="s">
         <v>81</v>
       </c>
@@ -3853,7 +3842,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A52" s="26" t="s">
         <v>82</v>
       </c>
@@ -3894,7 +3883,7 @@
       <c r="Z52" s="1"/>
       <c r="AA52" s="3"/>
     </row>
-    <row r="53" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A53" s="27" t="s">
         <v>84</v>
       </c>
@@ -3935,7 +3924,7 @@
       <c r="Z53" s="1"/>
       <c r="AA53" s="3"/>
     </row>
-    <row r="54" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A54" s="28" t="s">
         <v>86</v>
       </c>
@@ -3976,7 +3965,7 @@
       <c r="Z54" s="1"/>
       <c r="AA54" s="3"/>
     </row>
-    <row r="55" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A55" s="28" t="s">
         <v>86</v>
       </c>
@@ -4017,7 +4006,7 @@
       <c r="Z55" s="1"/>
       <c r="AA55" s="3"/>
     </row>
-    <row r="56" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A56" s="28" t="s">
         <v>86</v>
       </c>
@@ -4062,7 +4051,7 @@
       <c r="Z56" s="1"/>
       <c r="AA56" s="3"/>
     </row>
-    <row r="57" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A57" s="29" t="s">
         <v>90</v>
       </c>
@@ -4105,7 +4094,7 @@
       <c r="Z57" s="1"/>
       <c r="AA57" s="3"/>
     </row>
-    <row r="58" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A58" s="27" t="s">
         <v>92</v>
       </c>
@@ -4144,7 +4133,7 @@
       <c r="Z58" s="1"/>
       <c r="AA58" s="3"/>
     </row>
-    <row r="59" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A59" s="27" t="s">
         <v>92</v>
       </c>
@@ -4191,7 +4180,7 @@
       <c r="Z59" s="1"/>
       <c r="AA59" s="3"/>
     </row>
-    <row r="60" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A60" s="27" t="s">
         <v>92</v>
       </c>
@@ -4236,7 +4225,7 @@
       <c r="Z60" s="1"/>
       <c r="AA60" s="3"/>
     </row>
-    <row r="61" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A61" s="30" t="s">
         <v>94</v>
       </c>
@@ -4275,7 +4264,7 @@
       <c r="Z61" s="1"/>
       <c r="AA61" s="3"/>
     </row>
-    <row r="62" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A62" s="31" t="s">
         <v>98</v>
       </c>
@@ -4314,7 +4303,7 @@
       <c r="Z62" s="1"/>
       <c r="AA62" s="3"/>
     </row>
-    <row r="63" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A63" s="32" t="s">
         <v>100</v>
       </c>
@@ -4355,7 +4344,7 @@
       <c r="Z63" s="1"/>
       <c r="AA63" s="3"/>
     </row>
-    <row r="64" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A64" s="33" t="s">
         <v>102</v>
       </c>
@@ -4398,12 +4387,12 @@
       <c r="Z64" s="1"/>
       <c r="AA64" s="3"/>
     </row>
-    <row r="65" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="108" t="e">
+    <row r="65" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A65" s="109" t="e">
         <f>+B38:AA68</f>
         <v>#VALUE!</v>
       </c>
-      <c r="B65" s="109"/>
+      <c r="B65" s="110"/>
       <c r="C65" s="35" t="s">
         <v>42</v>
       </c>
@@ -4423,28 +4412,28 @@
         <f>COUNTIF(G5:G64, "X")</f>
         <v>26</v>
       </c>
-      <c r="H65" s="110"/>
-      <c r="I65" s="110"/>
-      <c r="J65" s="110"/>
-      <c r="K65" s="110"/>
-      <c r="L65" s="110"/>
-      <c r="M65" s="110"/>
-      <c r="N65" s="110"/>
-      <c r="O65" s="110"/>
-      <c r="P65" s="110"/>
-      <c r="Q65" s="110"/>
-      <c r="R65" s="110"/>
-      <c r="S65" s="110"/>
-      <c r="T65" s="110"/>
-      <c r="U65" s="110"/>
-      <c r="V65" s="110"/>
-      <c r="W65" s="110"/>
-      <c r="X65" s="110"/>
-      <c r="Y65" s="110"/>
-      <c r="Z65" s="110"/>
-      <c r="AA65" s="111"/>
-    </row>
-    <row r="66" spans="1:27" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+      <c r="H65" s="111"/>
+      <c r="I65" s="111"/>
+      <c r="J65" s="111"/>
+      <c r="K65" s="111"/>
+      <c r="L65" s="111"/>
+      <c r="M65" s="111"/>
+      <c r="N65" s="111"/>
+      <c r="O65" s="111"/>
+      <c r="P65" s="111"/>
+      <c r="Q65" s="111"/>
+      <c r="R65" s="111"/>
+      <c r="S65" s="111"/>
+      <c r="T65" s="111"/>
+      <c r="U65" s="111"/>
+      <c r="V65" s="111"/>
+      <c r="W65" s="111"/>
+      <c r="X65" s="111"/>
+      <c r="Y65" s="111"/>
+      <c r="Z65" s="111"/>
+      <c r="AA65" s="112"/>
+    </row>
+    <row r="66" spans="1:27" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="11">
     <mergeCell ref="A65:B65"/>

</xml_diff>

<commit_message>
Menu bases READ DESC for more info
-Had to modify libscreen.c as it uses global varaibles to store things, so i had to duplicate many functions to be able to create a separate screen for menu
-Right now you can print the menu, and do things with it, this afternoon i finish it and make it do things
</commit_message>
<xml_diff>
--- a/Reuniones_Coordinacion/Diagrama_Gantt_8_4_25_Saul_Fernando_Raquel_Irene.xlsx
+++ b/Reuniones_Coordinacion/Diagrama_Gantt_8_4_25_Saul_Fernando_Raquel_Irene.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\saul\Pprog_conversation\Reuniones_Coordinacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\fernandpo\cosa_uni\proyecto_program\Reuniones_Coordinacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B0C54B4-6490-4493-BDD1-A802A3F51C28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F539387B-2CC1-44FB-90F2-10739D2177A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{76F30C29-DD84-4491-9B4C-00A38B383DA8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{76F30C29-DD84-4491-9B4C-00A38B383DA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,17 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1384,9 +1395,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1424,7 +1435,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1530,7 +1541,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1672,7 +1683,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1682,22 +1693,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13B8C02F-838E-4995-8CF9-185661B72170}">
   <dimension ref="A1:AA66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="135" workbookViewId="0">
-      <selection activeCell="E58" sqref="E58"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="120" zoomScaleNormal="135" workbookViewId="0">
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="3.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="3.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="24" width="3" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="2.90625" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="2.88671875" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:27" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="113" t="s">
         <v>0</v>
       </c>
@@ -1728,7 +1739,7 @@
       <c r="Z1" s="114"/>
       <c r="AA1" s="115"/>
     </row>
-    <row r="2" spans="1:27" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:27" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="116" t="s">
         <v>1</v>
       </c>
@@ -1765,7 +1776,7 @@
       <c r="Z2" s="125"/>
       <c r="AA2" s="130"/>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" s="118"/>
       <c r="B3" s="119"/>
       <c r="C3" s="123"/>
@@ -1802,7 +1813,7 @@
       <c r="Z3" s="127"/>
       <c r="AA3" s="132"/>
     </row>
-    <row r="4" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="120"/>
       <c r="B4" s="121"/>
       <c r="C4" s="124"/>
@@ -1879,7 +1890,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:27" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A5" s="59" t="s">
         <v>13</v>
       </c>
@@ -1922,7 +1933,7 @@
       <c r="Z5" s="64"/>
       <c r="AA5" s="65"/>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
@@ -1961,7 +1972,7 @@
       <c r="Z6" s="71"/>
       <c r="AA6" s="17"/>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
@@ -2004,7 +2015,7 @@
       <c r="Z7" s="71"/>
       <c r="AA7" s="17"/>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
@@ -2047,7 +2058,7 @@
       <c r="Z8" s="71"/>
       <c r="AA8" s="17"/>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>20</v>
       </c>
@@ -2098,7 +2109,7 @@
       <c r="Z9" s="72"/>
       <c r="AA9" s="17"/>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>20</v>
       </c>
@@ -2143,7 +2154,7 @@
       <c r="Z10" s="72"/>
       <c r="AA10" s="17"/>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>23</v>
       </c>
@@ -2182,7 +2193,7 @@
       <c r="Z11" s="15"/>
       <c r="AA11" s="17"/>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>23</v>
       </c>
@@ -2221,7 +2232,7 @@
       <c r="Z12" s="15"/>
       <c r="AA12" s="17"/>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A13" s="18" t="s">
         <v>24</v>
       </c>
@@ -2260,7 +2271,7 @@
       <c r="Z13" s="15"/>
       <c r="AA13" s="17"/>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
         <v>24</v>
       </c>
@@ -2299,7 +2310,7 @@
       <c r="Z14" s="15"/>
       <c r="AA14" s="17"/>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A15" s="18" t="s">
         <v>24</v>
       </c>
@@ -2338,7 +2349,7 @@
       <c r="Z15" s="15"/>
       <c r="AA15" s="17"/>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A16" s="19" t="s">
         <v>25</v>
       </c>
@@ -2377,7 +2388,7 @@
       <c r="Z16" s="15"/>
       <c r="AA16" s="17"/>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A17" s="19" t="s">
         <v>25</v>
       </c>
@@ -2416,7 +2427,7 @@
       <c r="Z17" s="15"/>
       <c r="AA17" s="17"/>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A18" s="77" t="s">
         <v>26</v>
       </c>
@@ -2455,7 +2466,7 @@
       <c r="Z18" s="15"/>
       <c r="AA18" s="17"/>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A19" s="77" t="s">
         <v>26</v>
       </c>
@@ -2496,7 +2507,7 @@
       <c r="Z19" s="15"/>
       <c r="AA19" s="17"/>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A20" s="77" t="s">
         <v>26</v>
       </c>
@@ -2537,7 +2548,7 @@
       <c r="Z20" s="15"/>
       <c r="AA20" s="17"/>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A21" s="77" t="s">
         <v>26</v>
       </c>
@@ -2580,7 +2591,7 @@
       <c r="Z21" s="15"/>
       <c r="AA21" s="17"/>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>27</v>
       </c>
@@ -2619,7 +2630,7 @@
       <c r="Z22" s="15"/>
       <c r="AA22" s="17"/>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>27</v>
       </c>
@@ -2658,7 +2669,7 @@
       <c r="Z23" s="15"/>
       <c r="AA23" s="17"/>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>27</v>
       </c>
@@ -2703,7 +2714,7 @@
       <c r="Z24" s="15"/>
       <c r="AA24" s="17"/>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
         <v>28</v>
       </c>
@@ -2742,7 +2753,7 @@
       <c r="Z25" s="15"/>
       <c r="AA25" s="17"/>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
         <v>28</v>
       </c>
@@ -2781,7 +2792,7 @@
       <c r="Z26" s="15"/>
       <c r="AA26" s="17"/>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
         <v>28</v>
       </c>
@@ -2820,7 +2831,7 @@
       <c r="Z27" s="15"/>
       <c r="AA27" s="17"/>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A28" s="80" t="s">
         <v>29</v>
       </c>
@@ -2863,7 +2874,7 @@
       <c r="Z28" s="15"/>
       <c r="AA28" s="17"/>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
         <v>30</v>
       </c>
@@ -2904,7 +2915,7 @@
       <c r="Z29" s="15"/>
       <c r="AA29" s="17"/>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
         <v>30</v>
       </c>
@@ -2945,7 +2956,7 @@
       <c r="Z30" s="15"/>
       <c r="AA30" s="17"/>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A31" s="8" t="s">
         <v>31</v>
       </c>
@@ -2984,7 +2995,7 @@
       <c r="Z31" s="15"/>
       <c r="AA31" s="17"/>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A32" s="18" t="s">
         <v>32</v>
       </c>
@@ -3027,7 +3038,7 @@
       <c r="Z32" s="15"/>
       <c r="AA32" s="17"/>
     </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A33" s="18" t="s">
         <v>32</v>
       </c>
@@ -3074,7 +3085,7 @@
       <c r="Z33" s="15"/>
       <c r="AA33" s="17"/>
     </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="s">
         <v>33</v>
       </c>
@@ -3085,7 +3096,7 @@
         <v>64</v>
       </c>
       <c r="D34" s="15"/>
-      <c r="E34" s="15" t="s">
+      <c r="E34" s="106" t="s">
         <v>15</v>
       </c>
       <c r="F34" s="15"/>
@@ -3111,7 +3122,7 @@
       <c r="Z34" s="15"/>
       <c r="AA34" s="17"/>
     </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A35" s="10" t="s">
         <v>33</v>
       </c>
@@ -3122,7 +3133,7 @@
         <v>65</v>
       </c>
       <c r="D35" s="15"/>
-      <c r="E35" s="15" t="s">
+      <c r="E35" s="106" t="s">
         <v>15</v>
       </c>
       <c r="F35" s="15"/>
@@ -3152,7 +3163,7 @@
       <c r="Z35" s="15"/>
       <c r="AA35" s="17"/>
     </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A36" s="10" t="s">
         <v>33</v>
       </c>
@@ -3163,7 +3174,7 @@
         <v>66</v>
       </c>
       <c r="D36" s="15"/>
-      <c r="E36" s="15" t="s">
+      <c r="E36" s="106" t="s">
         <v>15</v>
       </c>
       <c r="F36" s="15"/>
@@ -3193,7 +3204,7 @@
       <c r="Z36" s="15"/>
       <c r="AA36" s="17"/>
     </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A37" s="10" t="s">
         <v>33</v>
       </c>
@@ -3204,7 +3215,7 @@
         <v>68</v>
       </c>
       <c r="D37" s="15"/>
-      <c r="E37" s="15" t="s">
+      <c r="E37" s="106" t="s">
         <v>15</v>
       </c>
       <c r="F37" s="15"/>
@@ -3238,7 +3249,7 @@
       <c r="Z37" s="15"/>
       <c r="AA37" s="17"/>
     </row>
-    <row r="38" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A38" s="10" t="s">
         <v>33</v>
       </c>
@@ -3251,7 +3262,7 @@
       <c r="D38" s="106" t="s">
         <v>15</v>
       </c>
-      <c r="E38" s="15" t="s">
+      <c r="E38" s="106" t="s">
         <v>15</v>
       </c>
       <c r="F38" s="15"/>
@@ -3285,7 +3296,7 @@
       <c r="Z38" s="15"/>
       <c r="AA38" s="17"/>
     </row>
-    <row r="39" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A39" s="9" t="s">
         <v>34</v>
       </c>
@@ -3326,7 +3337,7 @@
       <c r="Z39" s="15"/>
       <c r="AA39" s="17"/>
     </row>
-    <row r="40" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A40" s="9" t="s">
         <v>34</v>
       </c>
@@ -3371,7 +3382,7 @@
       <c r="Z40" s="15"/>
       <c r="AA40" s="17"/>
     </row>
-    <row r="41" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A41" s="9" t="s">
         <v>34</v>
       </c>
@@ -3416,7 +3427,7 @@
       <c r="Z41" s="15"/>
       <c r="AA41" s="17"/>
     </row>
-    <row r="42" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A42" s="9" t="s">
         <v>34</v>
       </c>
@@ -3465,7 +3476,7 @@
       <c r="Z42" s="15"/>
       <c r="AA42" s="17"/>
     </row>
-    <row r="43" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A43" s="20" t="s">
         <v>36</v>
       </c>
@@ -3504,7 +3515,7 @@
       <c r="Z43" s="15"/>
       <c r="AA43" s="17"/>
     </row>
-    <row r="44" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A44" s="21" t="s">
         <v>38</v>
       </c>
@@ -3547,7 +3558,7 @@
       <c r="Z44" s="15"/>
       <c r="AA44" s="17"/>
     </row>
-    <row r="45" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A45" s="21" t="s">
         <v>38</v>
       </c>
@@ -3590,7 +3601,7 @@
       <c r="Z45" s="15"/>
       <c r="AA45" s="17"/>
     </row>
-    <row r="46" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A46" s="21" t="s">
         <v>38</v>
       </c>
@@ -3629,7 +3640,7 @@
       <c r="Z46" s="15"/>
       <c r="AA46" s="17"/>
     </row>
-    <row r="47" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A47" s="10" t="s">
         <v>40</v>
       </c>
@@ -3674,7 +3685,7 @@
       <c r="Z47" s="15"/>
       <c r="AA47" s="17"/>
     </row>
-    <row r="48" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A48" s="24" t="s">
         <v>78</v>
       </c>
@@ -3717,7 +3728,7 @@
       <c r="Z48" s="70"/>
       <c r="AA48" s="17"/>
     </row>
-    <row r="49" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A49" s="11" t="s">
         <v>79</v>
       </c>
@@ -3760,7 +3771,7 @@
       <c r="Z49" s="23"/>
       <c r="AA49" s="25"/>
     </row>
-    <row r="50" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A50" s="12" t="s">
         <v>80</v>
       </c>
@@ -3803,7 +3814,7 @@
       <c r="Z50" s="88"/>
       <c r="AA50" s="89"/>
     </row>
-    <row r="51" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A51" s="13" t="s">
         <v>81</v>
       </c>
@@ -3842,7 +3853,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A52" s="26" t="s">
         <v>82</v>
       </c>
@@ -3883,7 +3894,7 @@
       <c r="Z52" s="1"/>
       <c r="AA52" s="3"/>
     </row>
-    <row r="53" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A53" s="27" t="s">
         <v>84</v>
       </c>
@@ -3924,7 +3935,7 @@
       <c r="Z53" s="1"/>
       <c r="AA53" s="3"/>
     </row>
-    <row r="54" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A54" s="28" t="s">
         <v>86</v>
       </c>
@@ -3935,7 +3946,7 @@
         <v>87</v>
       </c>
       <c r="D54" s="1"/>
-      <c r="E54" s="1" t="s">
+      <c r="E54" s="106" t="s">
         <v>15</v>
       </c>
       <c r="F54" s="1"/>
@@ -3965,7 +3976,7 @@
       <c r="Z54" s="1"/>
       <c r="AA54" s="3"/>
     </row>
-    <row r="55" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A55" s="28" t="s">
         <v>86</v>
       </c>
@@ -4006,7 +4017,7 @@
       <c r="Z55" s="1"/>
       <c r="AA55" s="3"/>
     </row>
-    <row r="56" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A56" s="28" t="s">
         <v>86</v>
       </c>
@@ -4051,7 +4062,7 @@
       <c r="Z56" s="1"/>
       <c r="AA56" s="3"/>
     </row>
-    <row r="57" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A57" s="29" t="s">
         <v>90</v>
       </c>
@@ -4094,7 +4105,7 @@
       <c r="Z57" s="1"/>
       <c r="AA57" s="3"/>
     </row>
-    <row r="58" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A58" s="27" t="s">
         <v>92</v>
       </c>
@@ -4133,7 +4144,7 @@
       <c r="Z58" s="1"/>
       <c r="AA58" s="3"/>
     </row>
-    <row r="59" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A59" s="27" t="s">
         <v>92</v>
       </c>
@@ -4180,7 +4191,7 @@
       <c r="Z59" s="1"/>
       <c r="AA59" s="3"/>
     </row>
-    <row r="60" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A60" s="27" t="s">
         <v>92</v>
       </c>
@@ -4225,7 +4236,7 @@
       <c r="Z60" s="1"/>
       <c r="AA60" s="3"/>
     </row>
-    <row r="61" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A61" s="30" t="s">
         <v>94</v>
       </c>
@@ -4264,7 +4275,7 @@
       <c r="Z61" s="1"/>
       <c r="AA61" s="3"/>
     </row>
-    <row r="62" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A62" s="31" t="s">
         <v>98</v>
       </c>
@@ -4303,7 +4314,7 @@
       <c r="Z62" s="1"/>
       <c r="AA62" s="3"/>
     </row>
-    <row r="63" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A63" s="32" t="s">
         <v>100</v>
       </c>
@@ -4344,7 +4355,7 @@
       <c r="Z63" s="1"/>
       <c r="AA63" s="3"/>
     </row>
-    <row r="64" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A64" s="33" t="s">
         <v>102</v>
       </c>
@@ -4387,7 +4398,7 @@
       <c r="Z64" s="1"/>
       <c r="AA64" s="3"/>
     </row>
-    <row r="65" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" s="109" t="e">
         <f>+B38:AA68</f>
         <v>#VALUE!</v>
@@ -4433,7 +4444,7 @@
       <c r="Z65" s="111"/>
       <c r="AA65" s="112"/>
     </row>
-    <row r="66" spans="1:27" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="66" spans="1:27" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="11">
     <mergeCell ref="A65:B65"/>

</xml_diff>